<commit_message>
add excel file with data
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="43480" yWindow="1660" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="whole_word_P_R_F1" sheetId="1" r:id="rId1"/>
@@ -135,8 +135,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="37">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -179,7 +191,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="37">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -198,6 +210,12 @@
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -216,6 +234,12 @@
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1067,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
+      <selection activeCell="E51" sqref="E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3348,8 +3372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M14" sqref="M14:M22"/>
+    <sheetView topLeftCell="A38" workbookViewId="0">
+      <selection activeCell="B27" sqref="B27:B35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3417,7 +3441,9 @@
       <c r="A3">
         <v>2608</v>
       </c>
-      <c r="B3" s="2"/>
+      <c r="B3">
+        <v>9</v>
+      </c>
       <c r="C3" s="2">
         <f>A3/$A$3</f>
         <v>1</v>
@@ -3425,7 +3451,9 @@
       <c r="D3">
         <v>2387</v>
       </c>
-      <c r="E3" s="2"/>
+      <c r="E3">
+        <v>9</v>
+      </c>
       <c r="F3" s="2">
         <f>D3/$D$3</f>
         <v>1</v>
@@ -3433,6 +3461,9 @@
       <c r="G3">
         <v>1902</v>
       </c>
+      <c r="H3">
+        <v>9</v>
+      </c>
       <c r="I3" s="2">
         <f>G3/$G$3</f>
         <v>1</v>
@@ -3440,12 +3471,18 @@
       <c r="J3">
         <v>2577</v>
       </c>
+      <c r="K3">
+        <v>9</v>
+      </c>
       <c r="L3" s="2">
         <f>J3/$J$3</f>
         <v>1</v>
       </c>
       <c r="M3">
         <v>2625</v>
+      </c>
+      <c r="N3">
+        <v>9</v>
       </c>
       <c r="O3" s="2">
         <f>M3/$M$3</f>
@@ -3456,7 +3493,9 @@
       <c r="A4" s="2">
         <v>2530</v>
       </c>
-      <c r="B4" s="2"/>
+      <c r="B4" s="2">
+        <v>8</v>
+      </c>
       <c r="C4" s="2">
         <f>A4/$A$3</f>
         <v>0.97009202453987731</v>
@@ -3464,7 +3503,9 @@
       <c r="D4" s="2">
         <v>2309</v>
       </c>
-      <c r="E4" s="2"/>
+      <c r="E4" s="2">
+        <v>8</v>
+      </c>
       <c r="F4" s="2">
         <f>D4/$D$3</f>
         <v>0.96732299958106405</v>
@@ -3472,7 +3513,9 @@
       <c r="G4" s="2">
         <v>1824</v>
       </c>
-      <c r="H4" s="2"/>
+      <c r="H4" s="2">
+        <v>8</v>
+      </c>
       <c r="I4" s="2">
         <f>G4/$G$3</f>
         <v>0.95899053627760256</v>
@@ -3480,7 +3523,9 @@
       <c r="J4" s="2">
         <v>2499</v>
       </c>
-      <c r="K4" s="2"/>
+      <c r="K4" s="2">
+        <v>8</v>
+      </c>
       <c r="L4" s="2">
         <f>J4/$J$3</f>
         <v>0.96973224679860304</v>
@@ -3488,7 +3533,9 @@
       <c r="M4" s="2">
         <v>2530</v>
       </c>
-      <c r="N4" s="2"/>
+      <c r="N4" s="2">
+        <v>8</v>
+      </c>
       <c r="O4" s="2">
         <f>M4/$M$3</f>
         <v>0.96380952380952378</v>
@@ -3498,7 +3545,9 @@
       <c r="A5" s="2">
         <v>2404</v>
       </c>
-      <c r="B5" s="2"/>
+      <c r="B5" s="2">
+        <v>7</v>
+      </c>
       <c r="C5" s="2">
         <f>A5/$A$3</f>
         <v>0.92177914110429449</v>
@@ -3506,7 +3555,9 @@
       <c r="D5" s="2">
         <v>2214</v>
       </c>
-      <c r="E5" s="2"/>
+      <c r="E5" s="2">
+        <v>7</v>
+      </c>
       <c r="F5" s="2">
         <f>D5/$D$3</f>
         <v>0.9275240888144114</v>
@@ -3514,7 +3565,9 @@
       <c r="G5" s="2">
         <v>1729</v>
       </c>
-      <c r="H5" s="2"/>
+      <c r="H5" s="2">
+        <v>7</v>
+      </c>
       <c r="I5" s="2">
         <f>G5/$G$3</f>
         <v>0.90904311251314407</v>
@@ -3522,7 +3575,9 @@
       <c r="J5" s="2">
         <v>2404</v>
       </c>
-      <c r="K5" s="2"/>
+      <c r="K5" s="2">
+        <v>7</v>
+      </c>
       <c r="L5" s="2">
         <f>J5/$J$3</f>
         <v>0.93286767559177342</v>
@@ -3530,7 +3585,9 @@
       <c r="M5" s="2">
         <v>2404</v>
       </c>
-      <c r="N5" s="2"/>
+      <c r="N5" s="2">
+        <v>7</v>
+      </c>
       <c r="O5" s="2">
         <f>M5/$M$3</f>
         <v>0.91580952380952385</v>
@@ -3540,7 +3597,9 @@
       <c r="A6" s="2">
         <v>2220</v>
       </c>
-      <c r="B6" s="2"/>
+      <c r="B6" s="2">
+        <v>6</v>
+      </c>
       <c r="C6" s="2">
         <f>A6/$A$3</f>
         <v>0.85122699386503065</v>
@@ -3548,7 +3607,9 @@
       <c r="D6" s="2">
         <v>2088</v>
       </c>
-      <c r="E6" s="2"/>
+      <c r="E6" s="2">
+        <v>6</v>
+      </c>
       <c r="F6" s="2">
         <f>D6/$D$3</f>
         <v>0.87473816506074575</v>
@@ -3556,7 +3617,9 @@
       <c r="G6" s="2">
         <v>1603</v>
       </c>
-      <c r="H6" s="2"/>
+      <c r="H6" s="2">
+        <v>6</v>
+      </c>
       <c r="I6" s="2">
         <f>G6/$G$3</f>
         <v>0.84279705573080965</v>
@@ -3564,7 +3627,9 @@
       <c r="J6" s="2">
         <v>2220</v>
       </c>
-      <c r="K6" s="2"/>
+      <c r="K6" s="2">
+        <v>6</v>
+      </c>
       <c r="L6" s="2">
         <f>J6/$J$3</f>
         <v>0.86146682188591384</v>
@@ -3572,7 +3637,9 @@
       <c r="M6" s="2">
         <v>2220</v>
       </c>
-      <c r="N6" s="2"/>
+      <c r="N6" s="2">
+        <v>6</v>
+      </c>
       <c r="O6" s="2">
         <f>M6/$M$3</f>
         <v>0.84571428571428575</v>
@@ -3582,7 +3649,9 @@
       <c r="A7" s="2">
         <v>2024</v>
       </c>
-      <c r="B7" s="2"/>
+      <c r="B7" s="2">
+        <v>5</v>
+      </c>
       <c r="C7" s="2">
         <f>A7/$A$3</f>
         <v>0.7760736196319018</v>
@@ -3590,7 +3659,9 @@
       <c r="D7" s="2">
         <v>1904</v>
       </c>
-      <c r="E7" s="2"/>
+      <c r="E7" s="2">
+        <v>5</v>
+      </c>
       <c r="F7" s="2">
         <f>D7/$D$3</f>
         <v>0.79765395894428148</v>
@@ -3598,7 +3669,9 @@
       <c r="G7" s="2">
         <v>1419</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2">
+        <v>5</v>
+      </c>
       <c r="I7" s="2">
         <f>G7/$G$3</f>
         <v>0.74605678233438488</v>
@@ -3606,7 +3679,9 @@
       <c r="J7" s="2">
         <v>2024</v>
       </c>
-      <c r="K7" s="2"/>
+      <c r="K7" s="2">
+        <v>5</v>
+      </c>
       <c r="L7" s="2">
         <f>J7/$J$3</f>
         <v>0.78540939076445482</v>
@@ -3614,7 +3689,9 @@
       <c r="M7" s="2">
         <v>2024</v>
       </c>
-      <c r="N7" s="2"/>
+      <c r="N7" s="2">
+        <v>5</v>
+      </c>
       <c r="O7" s="2">
         <f>M7/$M$3</f>
         <v>0.77104761904761909</v>
@@ -3624,7 +3701,9 @@
       <c r="A8" s="2">
         <v>1815</v>
       </c>
-      <c r="B8" s="2"/>
+      <c r="B8" s="2">
+        <v>4</v>
+      </c>
       <c r="C8" s="2">
         <f>A8/$A$3</f>
         <v>0.6959355828220859</v>
@@ -3632,7 +3711,9 @@
       <c r="D8" s="2">
         <v>1708</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2">
+        <v>4</v>
+      </c>
       <c r="F8" s="2">
         <f>D8/$D$3</f>
         <v>0.71554252199413493</v>
@@ -3640,7 +3721,9 @@
       <c r="G8" s="2">
         <v>1223</v>
       </c>
-      <c r="H8" s="2"/>
+      <c r="H8" s="2">
+        <v>4</v>
+      </c>
       <c r="I8" s="2">
         <f>G8/$G$3</f>
         <v>0.64300736067297581</v>
@@ -3648,7 +3731,9 @@
       <c r="J8" s="2">
         <v>1815</v>
       </c>
-      <c r="K8" s="2"/>
+      <c r="K8" s="2">
+        <v>4</v>
+      </c>
       <c r="L8" s="2">
         <f>J8/$J$3</f>
         <v>0.70430733410942958</v>
@@ -3656,7 +3741,9 @@
       <c r="M8" s="2">
         <v>1815</v>
       </c>
-      <c r="N8" s="2"/>
+      <c r="N8" s="2">
+        <v>4</v>
+      </c>
       <c r="O8" s="2">
         <f>M8/$M$3</f>
         <v>0.69142857142857139</v>
@@ -3666,7 +3753,9 @@
       <c r="A9" s="2">
         <v>1499</v>
       </c>
-      <c r="B9" s="2"/>
+      <c r="B9" s="2">
+        <v>3</v>
+      </c>
       <c r="C9" s="2">
         <f>A9/$A$3</f>
         <v>0.57476993865030679</v>
@@ -3674,7 +3763,9 @@
       <c r="D9" s="2">
         <v>1499</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2">
+        <v>3</v>
+      </c>
       <c r="F9" s="2">
         <f>D9/$D$3</f>
         <v>0.62798491830749892</v>
@@ -3682,7 +3773,9 @@
       <c r="G9" s="2">
         <v>1014</v>
       </c>
-      <c r="H9" s="2"/>
+      <c r="H9" s="2">
+        <v>3</v>
+      </c>
       <c r="I9" s="2">
         <f>G9/$G$3</f>
         <v>0.53312302839116721</v>
@@ -3690,7 +3783,9 @@
       <c r="J9" s="2">
         <v>1499</v>
       </c>
-      <c r="K9" s="2"/>
+      <c r="K9" s="2">
+        <v>3</v>
+      </c>
       <c r="L9" s="2">
         <f>J9/$J$3</f>
         <v>0.58168412883197518</v>
@@ -3698,7 +3793,9 @@
       <c r="M9" s="2">
         <v>1499</v>
       </c>
-      <c r="N9" s="2"/>
+      <c r="N9" s="2">
+        <v>3</v>
+      </c>
       <c r="O9" s="2">
         <f>M9/$M$3</f>
         <v>0.57104761904761903</v>
@@ -3708,7 +3805,9 @@
       <c r="A10" s="2">
         <v>1156</v>
       </c>
-      <c r="B10" s="2"/>
+      <c r="B10" s="2">
+        <v>2</v>
+      </c>
       <c r="C10" s="2">
         <f>A10/$A$3</f>
         <v>0.44325153374233128</v>
@@ -3716,7 +3815,9 @@
       <c r="D10" s="2">
         <v>1156</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2">
+        <v>2</v>
+      </c>
       <c r="F10" s="2">
         <f>D10/$D$3</f>
         <v>0.48428990364474234</v>
@@ -3724,7 +3825,9 @@
       <c r="G10" s="2">
         <v>698</v>
       </c>
-      <c r="H10" s="2"/>
+      <c r="H10" s="2">
+        <v>2</v>
+      </c>
       <c r="I10" s="2">
         <f>G10/$G$3</f>
         <v>0.36698212407991587</v>
@@ -3732,7 +3835,9 @@
       <c r="J10" s="2">
         <v>1156</v>
       </c>
-      <c r="K10" s="2"/>
+      <c r="K10" s="2">
+        <v>2</v>
+      </c>
       <c r="L10" s="2">
         <f>J10/$J$3</f>
         <v>0.44858362436942179</v>
@@ -3740,7 +3845,9 @@
       <c r="M10" s="2">
         <v>1156</v>
       </c>
-      <c r="N10" s="2"/>
+      <c r="N10" s="2">
+        <v>2</v>
+      </c>
       <c r="O10" s="2">
         <f>M10/$M$3</f>
         <v>0.44038095238095237</v>
@@ -3750,7 +3857,9 @@
       <c r="A11" s="2">
         <v>801</v>
       </c>
-      <c r="B11" s="2"/>
+      <c r="B11" s="2">
+        <v>1</v>
+      </c>
       <c r="C11" s="2">
         <f>A11/$A$3</f>
         <v>0.30713190184049077</v>
@@ -3758,7 +3867,9 @@
       <c r="D11" s="2">
         <v>801</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2">
+        <v>1</v>
+      </c>
       <c r="F11" s="2">
         <f>D11/$D$3</f>
         <v>0.3355676581483033</v>
@@ -3766,7 +3877,9 @@
       <c r="G11" s="2">
         <v>355</v>
       </c>
-      <c r="H11" s="2"/>
+      <c r="H11" s="2">
+        <v>1</v>
+      </c>
       <c r="I11" s="2">
         <f>G11/$G$3</f>
         <v>0.18664563617245006</v>
@@ -3774,7 +3887,9 @@
       <c r="J11" s="2">
         <v>801</v>
       </c>
-      <c r="K11" s="2"/>
+      <c r="K11" s="2">
+        <v>1</v>
+      </c>
       <c r="L11" s="2">
         <f>J11/$J$3</f>
         <v>0.3108265424912689</v>
@@ -3782,7 +3897,9 @@
       <c r="M11" s="2">
         <v>801</v>
       </c>
-      <c r="N11" s="2"/>
+      <c r="N11" s="2">
+        <v>1</v>
+      </c>
       <c r="O11" s="2">
         <f>M11/$M$3</f>
         <v>0.30514285714285716</v>
@@ -3856,7 +3973,9 @@
       <c r="A14" s="2">
         <v>2348</v>
       </c>
-      <c r="B14" s="2"/>
+      <c r="B14">
+        <v>9</v>
+      </c>
       <c r="C14" s="2">
         <f>A14/$A$14</f>
         <v>1</v>
@@ -3864,7 +3983,9 @@
       <c r="D14" s="2">
         <v>2507</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14">
+        <v>9</v>
+      </c>
       <c r="F14" s="2">
         <f>D14/$D$14</f>
         <v>1</v>
@@ -3872,7 +3993,9 @@
       <c r="G14" s="2">
         <v>2519</v>
       </c>
-      <c r="H14" s="2"/>
+      <c r="H14">
+        <v>9</v>
+      </c>
       <c r="I14" s="2">
         <f>G14/$G$14</f>
         <v>1</v>
@@ -3880,7 +4003,9 @@
       <c r="J14" s="2">
         <v>2360</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14">
+        <v>9</v>
+      </c>
       <c r="L14" s="2">
         <f>J14/$J$14</f>
         <v>1</v>
@@ -3888,7 +4013,9 @@
       <c r="M14" s="2">
         <v>2494</v>
       </c>
-      <c r="N14" s="2"/>
+      <c r="N14">
+        <v>9</v>
+      </c>
       <c r="O14" s="2">
         <f>M14/$M$14</f>
         <v>1</v>
@@ -3898,7 +4025,9 @@
       <c r="A15" s="2">
         <v>2270</v>
       </c>
-      <c r="B15" s="2"/>
+      <c r="B15" s="2">
+        <v>8</v>
+      </c>
       <c r="C15" s="2">
         <f t="shared" ref="C15:C22" si="0">A15/$A$14</f>
         <v>0.96678023850085182</v>
@@ -3906,7 +4035,9 @@
       <c r="D15" s="2">
         <v>2429</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2">
+        <v>8</v>
+      </c>
       <c r="F15" s="2">
         <f t="shared" ref="F15:F22" si="1">D15/$D$14</f>
         <v>0.96888711607499001</v>
@@ -3914,7 +4045,9 @@
       <c r="G15" s="2">
         <v>2441</v>
       </c>
-      <c r="H15" s="2"/>
+      <c r="H15" s="2">
+        <v>8</v>
+      </c>
       <c r="I15" s="2">
         <f t="shared" ref="I15:I22" si="2">G15/$G$14</f>
         <v>0.96903533148074628</v>
@@ -3922,7 +4055,9 @@
       <c r="J15" s="2">
         <v>2282</v>
       </c>
-      <c r="K15" s="2"/>
+      <c r="K15" s="2">
+        <v>8</v>
+      </c>
       <c r="L15" s="2">
         <f t="shared" ref="L15:L22" si="3">J15/$J$14</f>
         <v>0.9669491525423729</v>
@@ -3930,7 +4065,9 @@
       <c r="M15" s="2">
         <v>2416</v>
       </c>
-      <c r="N15" s="2"/>
+      <c r="N15" s="2">
+        <v>8</v>
+      </c>
       <c r="O15" s="2">
         <f>M15/$M$14</f>
         <v>0.96872493985565356</v>
@@ -3940,7 +4077,9 @@
       <c r="A16" s="2">
         <v>2175</v>
       </c>
-      <c r="B16" s="2"/>
+      <c r="B16" s="2">
+        <v>7</v>
+      </c>
       <c r="C16" s="2">
         <f t="shared" si="0"/>
         <v>0.92632027257240201</v>
@@ -3948,7 +4087,9 @@
       <c r="D16" s="2">
         <v>2334</v>
       </c>
-      <c r="E16" s="2"/>
+      <c r="E16" s="2">
+        <v>7</v>
+      </c>
       <c r="F16" s="2">
         <f t="shared" si="1"/>
         <v>0.93099321898683685</v>
@@ -3956,7 +4097,9 @@
       <c r="G16" s="2">
         <v>2346</v>
       </c>
-      <c r="H16" s="2"/>
+      <c r="H16" s="2">
+        <v>7</v>
+      </c>
       <c r="I16" s="2">
         <f t="shared" si="2"/>
         <v>0.93132195315601429</v>
@@ -3964,7 +4107,9 @@
       <c r="J16" s="2">
         <v>2187</v>
       </c>
-      <c r="K16" s="2"/>
+      <c r="K16" s="2">
+        <v>7</v>
+      </c>
       <c r="L16" s="2">
         <f t="shared" si="3"/>
         <v>0.92669491525423731</v>
@@ -3972,7 +4117,9 @@
       <c r="M16" s="2">
         <v>2321</v>
       </c>
-      <c r="N16" s="2"/>
+      <c r="N16" s="2">
+        <v>7</v>
+      </c>
       <c r="O16" s="2">
         <f>M16/$M$14</f>
         <v>0.93063352044907777</v>
@@ -3982,7 +4129,9 @@
       <c r="A17" s="2">
         <v>2049</v>
       </c>
-      <c r="B17" s="2"/>
+      <c r="B17" s="2">
+        <v>6</v>
+      </c>
       <c r="C17" s="2">
         <f t="shared" si="0"/>
         <v>0.87265758091993184</v>
@@ -3990,7 +4139,9 @@
       <c r="D17" s="2">
         <v>2208</v>
       </c>
-      <c r="E17" s="2"/>
+      <c r="E17" s="2">
+        <v>6</v>
+      </c>
       <c r="F17" s="2">
         <f t="shared" si="1"/>
         <v>0.88073394495412849</v>
@@ -3998,7 +4149,9 @@
       <c r="G17" s="2">
         <v>2220</v>
       </c>
-      <c r="H17" s="2"/>
+      <c r="H17" s="2">
+        <v>6</v>
+      </c>
       <c r="I17" s="2">
         <f t="shared" si="2"/>
         <v>0.88130210400952758</v>
@@ -4006,7 +4159,9 @@
       <c r="J17" s="2">
         <v>2061</v>
       </c>
-      <c r="K17" s="2"/>
+      <c r="K17" s="2">
+        <v>6</v>
+      </c>
       <c r="L17" s="2">
         <f t="shared" si="3"/>
         <v>0.87330508474576274</v>
@@ -4014,7 +4169,9 @@
       <c r="M17" s="2">
         <v>2195</v>
       </c>
-      <c r="N17" s="2"/>
+      <c r="N17" s="2">
+        <v>6</v>
+      </c>
       <c r="O17" s="2">
         <f>M17/$M$14</f>
         <v>0.88011226944667198</v>
@@ -4024,7 +4181,9 @@
       <c r="A18" s="2">
         <v>1865</v>
       </c>
-      <c r="B18" s="2"/>
+      <c r="B18" s="2">
+        <v>5</v>
+      </c>
       <c r="C18" s="2">
         <f t="shared" si="0"/>
         <v>0.79429301533219765</v>
@@ -4032,7 +4191,9 @@
       <c r="D18" s="2">
         <v>2024</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="2">
+        <v>5</v>
+      </c>
       <c r="F18" s="2">
         <f t="shared" si="1"/>
         <v>0.80733944954128445</v>
@@ -4040,7 +4201,9 @@
       <c r="G18" s="2">
         <v>2024</v>
       </c>
-      <c r="H18" s="2"/>
+      <c r="H18" s="2">
+        <v>5</v>
+      </c>
       <c r="I18" s="2">
         <f t="shared" si="2"/>
         <v>0.80349344978165937</v>
@@ -4048,7 +4211,9 @@
       <c r="J18" s="2">
         <v>1877</v>
       </c>
-      <c r="K18" s="2"/>
+      <c r="K18" s="2">
+        <v>5</v>
+      </c>
       <c r="L18" s="2">
         <f t="shared" si="3"/>
         <v>0.79533898305084749</v>
@@ -4056,7 +4221,9 @@
       <c r="M18" s="2">
         <v>2011</v>
       </c>
-      <c r="N18" s="2"/>
+      <c r="N18" s="2">
+        <v>5</v>
+      </c>
       <c r="O18" s="2">
         <f>M18/$M$14</f>
         <v>0.80633520449077789</v>
@@ -4066,7 +4233,9 @@
       <c r="A19" s="2">
         <v>1669</v>
       </c>
-      <c r="B19" s="2"/>
+      <c r="B19" s="2">
+        <v>4</v>
+      </c>
       <c r="C19" s="2">
         <f t="shared" si="0"/>
         <v>0.71081771720613285</v>
@@ -4074,7 +4243,9 @@
       <c r="D19" s="2">
         <v>1815</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="2">
+        <v>4</v>
+      </c>
       <c r="F19" s="2">
         <f t="shared" si="1"/>
         <v>0.72397287594734738</v>
@@ -4082,7 +4253,9 @@
       <c r="G19" s="2">
         <v>1815</v>
       </c>
-      <c r="H19" s="2"/>
+      <c r="H19" s="2">
+        <v>4</v>
+      </c>
       <c r="I19" s="2">
         <f t="shared" si="2"/>
         <v>0.72052401746724892</v>
@@ -4090,7 +4263,9 @@
       <c r="J19" s="2">
         <v>1681</v>
       </c>
-      <c r="K19" s="2"/>
+      <c r="K19" s="2">
+        <v>4</v>
+      </c>
       <c r="L19" s="2">
         <f t="shared" si="3"/>
         <v>0.71228813559322035</v>
@@ -4098,7 +4273,9 @@
       <c r="M19" s="2">
         <v>1815</v>
       </c>
-      <c r="N19" s="2"/>
+      <c r="N19" s="2">
+        <v>4</v>
+      </c>
       <c r="O19" s="2">
         <f>M19/$M$14</f>
         <v>0.72774659182036894</v>
@@ -4108,7 +4285,9 @@
       <c r="A20" s="2">
         <v>1460</v>
       </c>
-      <c r="B20" s="2"/>
+      <c r="B20" s="2">
+        <v>3</v>
+      </c>
       <c r="C20" s="2">
         <f t="shared" si="0"/>
         <v>0.62180579216354348</v>
@@ -4116,7 +4295,9 @@
       <c r="D20" s="2">
         <v>1499</v>
       </c>
-      <c r="E20" s="2"/>
+      <c r="E20" s="2">
+        <v>3</v>
+      </c>
       <c r="F20" s="2">
         <f t="shared" si="1"/>
         <v>0.5979258077383327</v>
@@ -4124,7 +4305,9 @@
       <c r="G20" s="2">
         <v>1499</v>
       </c>
-      <c r="H20" s="2"/>
+      <c r="H20" s="2">
+        <v>3</v>
+      </c>
       <c r="I20" s="2">
         <f t="shared" si="2"/>
         <v>0.59507741167129813</v>
@@ -4132,7 +4315,9 @@
       <c r="J20" s="2">
         <v>1472</v>
       </c>
-      <c r="K20" s="2"/>
+      <c r="K20" s="2">
+        <v>3</v>
+      </c>
       <c r="L20" s="2">
         <f t="shared" si="3"/>
         <v>0.62372881355932208</v>
@@ -4140,7 +4325,9 @@
       <c r="M20" s="2">
         <v>1499</v>
       </c>
-      <c r="N20" s="2"/>
+      <c r="N20" s="2">
+        <v>3</v>
+      </c>
       <c r="O20" s="2">
         <f>M20/$M$14</f>
         <v>0.60104250200481157</v>
@@ -4150,7 +4337,9 @@
       <c r="A21" s="2">
         <v>1144</v>
       </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="2">
+        <v>2</v>
+      </c>
       <c r="C21" s="2">
         <f t="shared" si="0"/>
         <v>0.48722316865417375</v>
@@ -4158,7 +4347,9 @@
       <c r="D21" s="2">
         <v>1156</v>
       </c>
-      <c r="E21" s="2"/>
+      <c r="E21" s="2">
+        <v>2</v>
+      </c>
       <c r="F21" s="2">
         <f t="shared" si="1"/>
         <v>0.46110889509373754</v>
@@ -4166,7 +4357,9 @@
       <c r="G21" s="2">
         <v>1156</v>
       </c>
-      <c r="H21" s="2"/>
+      <c r="H21" s="2">
+        <v>2</v>
+      </c>
       <c r="I21" s="2">
         <f t="shared" si="2"/>
         <v>0.45891226677252878</v>
@@ -4174,7 +4367,9 @@
       <c r="J21" s="2">
         <v>1156</v>
       </c>
-      <c r="K21" s="2"/>
+      <c r="K21" s="2">
+        <v>2</v>
+      </c>
       <c r="L21" s="2">
         <f t="shared" si="3"/>
         <v>0.48983050847457626</v>
@@ -4182,7 +4377,9 @@
       <c r="M21" s="2">
         <v>1156</v>
       </c>
-      <c r="N21" s="2"/>
+      <c r="N21" s="2">
+        <v>2</v>
+      </c>
       <c r="O21" s="2">
         <f>M21/$M$14</f>
         <v>0.46351242983159585</v>
@@ -4192,7 +4389,9 @@
       <c r="A22" s="2">
         <v>801</v>
       </c>
-      <c r="B22" s="2"/>
+      <c r="B22" s="2">
+        <v>1</v>
+      </c>
       <c r="C22" s="2">
         <f t="shared" si="0"/>
         <v>0.34114139693356049</v>
@@ -4200,7 +4399,9 @@
       <c r="D22" s="2">
         <v>801</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="2">
+        <v>1</v>
+      </c>
       <c r="F22" s="2">
         <f t="shared" si="1"/>
         <v>0.31950538492221781</v>
@@ -4208,7 +4409,9 @@
       <c r="G22" s="2">
         <v>801</v>
       </c>
-      <c r="H22" s="2"/>
+      <c r="H22" s="2">
+        <v>1</v>
+      </c>
       <c r="I22" s="2">
         <f t="shared" si="2"/>
         <v>0.31798332671695118</v>
@@ -4216,7 +4419,9 @@
       <c r="J22" s="2">
         <v>801</v>
       </c>
-      <c r="K22" s="2"/>
+      <c r="K22" s="2">
+        <v>1</v>
+      </c>
       <c r="L22" s="2">
         <f t="shared" si="3"/>
         <v>0.33940677966101696</v>
@@ -4224,7 +4429,9 @@
       <c r="M22" s="2">
         <v>801</v>
       </c>
-      <c r="N22" s="2"/>
+      <c r="N22" s="2">
+        <v>1</v>
+      </c>
       <c r="O22" s="2">
         <f>M22/$M$14</f>
         <v>0.32117080994386527</v>
@@ -4239,45 +4446,72 @@
       <c r="A27">
         <v>1</v>
       </c>
+      <c r="B27">
+        <v>756</v>
+      </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28">
         <v>2</v>
       </c>
+      <c r="B28">
+        <v>1106</v>
+      </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29">
         <v>3</v>
       </c>
+      <c r="B29">
+        <v>1444</v>
+      </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30">
         <v>4</v>
       </c>
+      <c r="B30">
+        <v>1717</v>
+      </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31">
         <v>5</v>
       </c>
+      <c r="B31">
+        <v>1919</v>
+      </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32">
         <v>6</v>
       </c>
+      <c r="B32">
+        <v>2108</v>
+      </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33">
         <v>7</v>
       </c>
+      <c r="B33">
+        <v>2251</v>
+      </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34">
         <v>8</v>
       </c>
+      <c r="B34">
+        <v>2353</v>
+      </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35">
         <v>9</v>
+      </c>
+      <c r="B35">
+        <v>2432</v>
       </c>
     </row>
     <row r="38" spans="1:15">

</xml_diff>

<commit_message>
add more arguments to rqiii
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="43480" yWindow="1660" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="43480" yWindow="1660" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="whole_word_P_R_F1" sheetId="1" r:id="rId1"/>
@@ -1091,8 +1091,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A35" workbookViewId="0">
-      <selection activeCell="E51" sqref="E51"/>
+    <sheetView topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="A66" sqref="A66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3372,8 +3372,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView topLeftCell="A38" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27:B35"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="C70" sqref="C70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5575,43 +5575,52 @@
       <c r="A63">
         <v>1</v>
       </c>
+      <c r="B63">
+        <v>600</v>
+      </c>
     </row>
     <row r="64" spans="1:15">
       <c r="A64">
         <v>2</v>
       </c>
     </row>
-    <row r="65" spans="1:1">
+    <row r="65" spans="1:2">
       <c r="A65">
         <v>3</v>
       </c>
     </row>
-    <row r="66" spans="1:1">
+    <row r="66" spans="1:2">
       <c r="A66">
         <v>4</v>
       </c>
-    </row>
-    <row r="67" spans="1:1">
+      <c r="B66">
+        <v>1023</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2">
       <c r="A67">
         <v>5</v>
       </c>
     </row>
-    <row r="68" spans="1:1">
+    <row r="68" spans="1:2">
       <c r="A68">
         <v>6</v>
       </c>
     </row>
-    <row r="69" spans="1:1">
+    <row r="69" spans="1:2">
       <c r="A69">
         <v>7</v>
       </c>
-    </row>
-    <row r="70" spans="1:1">
+      <c r="B69">
+        <v>1055</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2">
       <c r="A70">
         <v>8</v>
       </c>
     </row>
-    <row r="71" spans="1:1">
+    <row r="71" spans="1:2">
       <c r="A71">
         <v>9</v>
       </c>

</xml_diff>

<commit_message>
address comments untill discussion
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="45880" yWindow="2400" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="45880" yWindow="2400" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="whole_word_P_R_F1" sheetId="1" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="30">
   <si>
     <t>design</t>
   </si>
@@ -108,6 +108,12 @@
   <si>
     <t>average</t>
   </si>
+  <si>
+    <t>delta design</t>
+  </si>
+  <si>
+    <t>delta requirement</t>
+  </si>
 </sst>
 </file>
 
@@ -155,8 +161,42 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="103">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -265,7 +305,7 @@
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="103">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -317,6 +357,23 @@
     <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -368,6 +425,23 @@
     <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1219,8 +1293,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="J63" sqref="J63:J71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2284,6 +2358,9 @@
       <c r="A26" t="s">
         <v>15</v>
       </c>
+      <c r="I26" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="27" spans="1:15">
       <c r="A27">
@@ -2299,6 +2376,13 @@
         <f>C27/$C$33</f>
         <v>0.31085526315789475</v>
       </c>
+      <c r="I27">
+        <v>0.71799999999999997</v>
+      </c>
+      <c r="J27">
+        <f>I28-I27</f>
+        <v>0.13800000000000001</v>
+      </c>
     </row>
     <row r="28" spans="1:15">
       <c r="A28">
@@ -2314,6 +2398,13 @@
         <f t="shared" ref="D28:D35" si="10">C28/$C$33</f>
         <v>0.45476973684210525</v>
       </c>
+      <c r="I28">
+        <v>0.85599999999999998</v>
+      </c>
+      <c r="J28">
+        <f t="shared" ref="J28:J35" si="11">I29-I28</f>
+        <v>6.800000000000006E-2</v>
+      </c>
     </row>
     <row r="29" spans="1:15">
       <c r="A29">
@@ -2329,6 +2420,13 @@
         <f t="shared" si="10"/>
         <v>0.70600328947368418</v>
       </c>
+      <c r="I29">
+        <v>0.92400000000000004</v>
+      </c>
+      <c r="J29">
+        <f t="shared" si="11"/>
+        <v>-1.2000000000000011E-2</v>
+      </c>
     </row>
     <row r="30" spans="1:15">
       <c r="A30">
@@ -2344,6 +2442,13 @@
         <f t="shared" si="10"/>
         <v>0.59375</v>
       </c>
+      <c r="I30">
+        <v>0.91200000000000003</v>
+      </c>
+      <c r="J30">
+        <f t="shared" si="11"/>
+        <v>1.5000000000000013E-2</v>
+      </c>
     </row>
     <row r="31" spans="1:15">
       <c r="A31">
@@ -2359,6 +2464,13 @@
         <f t="shared" si="10"/>
         <v>0.7890625</v>
       </c>
+      <c r="I31">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="J31">
+        <f t="shared" si="11"/>
+        <v>3.0000000000000027E-3</v>
+      </c>
     </row>
     <row r="32" spans="1:15">
       <c r="A32">
@@ -2374,6 +2486,13 @@
         <f t="shared" si="10"/>
         <v>0.86677631578947367</v>
       </c>
+      <c r="I32">
+        <v>0.93</v>
+      </c>
+      <c r="J32">
+        <f t="shared" si="11"/>
+        <v>3.2999999999999918E-2</v>
+      </c>
     </row>
     <row r="33" spans="1:15">
       <c r="A33">
@@ -2389,6 +2508,13 @@
         <f t="shared" si="10"/>
         <v>1</v>
       </c>
+      <c r="I33">
+        <v>0.96299999999999997</v>
+      </c>
+      <c r="J33">
+        <f t="shared" si="11"/>
+        <v>2.0000000000000018E-3</v>
+      </c>
     </row>
     <row r="34" spans="1:15">
       <c r="A34">
@@ -2404,6 +2530,13 @@
         <f t="shared" si="10"/>
         <v>0.92557565789473684</v>
       </c>
+      <c r="I34">
+        <v>0.96499999999999997</v>
+      </c>
+      <c r="J34">
+        <f t="shared" si="11"/>
+        <v>-6.0000000000000053E-3</v>
+      </c>
     </row>
     <row r="35" spans="1:15">
       <c r="A35">
@@ -2419,6 +2552,13 @@
         <f t="shared" si="10"/>
         <v>0.96751644736842102</v>
       </c>
+      <c r="I35">
+        <v>0.95899999999999996</v>
+      </c>
+      <c r="J35">
+        <f t="shared" si="11"/>
+        <v>-0.95899999999999996</v>
+      </c>
     </row>
     <row r="38" spans="1:15">
       <c r="A38" t="s">
@@ -2480,7 +2620,7 @@
         <v>7</v>
       </c>
       <c r="C40" s="2">
-        <f t="shared" ref="C40:C48" si="11">A40/$A$40</f>
+        <f t="shared" ref="C40:C48" si="12">A40/$A$40</f>
         <v>1</v>
       </c>
       <c r="D40">
@@ -2532,7 +2672,7 @@
         <v>8</v>
       </c>
       <c r="C41" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="D41" s="2">
@@ -2542,7 +2682,7 @@
         <v>4</v>
       </c>
       <c r="F41" s="2">
-        <f t="shared" ref="F41:F48" si="12">D41/$D$40</f>
+        <f t="shared" ref="F41:F48" si="13">D41/$D$40</f>
         <v>0.92901234567901225</v>
       </c>
       <c r="G41" s="2">
@@ -2552,7 +2692,7 @@
         <v>8</v>
       </c>
       <c r="I41" s="2">
-        <f t="shared" ref="I41:I48" si="13">G41/$G$40</f>
+        <f t="shared" ref="I41:I48" si="14">G41/$G$40</f>
         <v>0.99611398963730569</v>
       </c>
       <c r="J41" s="2">
@@ -2562,7 +2702,7 @@
         <v>6</v>
       </c>
       <c r="L41" s="2">
-        <f t="shared" ref="L41:L48" si="14">J41/$J$40</f>
+        <f t="shared" ref="L41:L48" si="15">J41/$J$40</f>
         <v>1</v>
       </c>
       <c r="M41" s="2">
@@ -2572,7 +2712,7 @@
         <v>7</v>
       </c>
       <c r="O41" s="2">
-        <f t="shared" ref="O41:O48" si="15">M41/$M$40</f>
+        <f t="shared" ref="O41:O48" si="16">M41/$M$40</f>
         <v>0.75065616797900259</v>
       </c>
     </row>
@@ -2584,7 +2724,7 @@
         <v>9</v>
       </c>
       <c r="C42" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>1</v>
       </c>
       <c r="D42" s="2">
@@ -2594,7 +2734,7 @@
         <v>1</v>
       </c>
       <c r="F42" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.91666666666666663</v>
       </c>
       <c r="G42" s="2">
@@ -2604,7 +2744,7 @@
         <v>9</v>
       </c>
       <c r="I42" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.98445595854922274</v>
       </c>
       <c r="J42" s="2">
@@ -2614,7 +2754,7 @@
         <v>7</v>
       </c>
       <c r="L42" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="M42" s="2">
@@ -2624,7 +2764,7 @@
         <v>4</v>
       </c>
       <c r="O42" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.75065616797900259</v>
       </c>
     </row>
@@ -2636,7 +2776,7 @@
         <v>3</v>
       </c>
       <c r="C43" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.51165146909827763</v>
       </c>
       <c r="D43" s="2">
@@ -2646,7 +2786,7 @@
         <v>3</v>
       </c>
       <c r="F43" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.8950617283950616</v>
       </c>
       <c r="G43" s="2">
@@ -2656,7 +2796,7 @@
         <v>6</v>
       </c>
       <c r="I43" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.97668393782383423</v>
       </c>
       <c r="J43" s="2">
@@ -2666,7 +2806,7 @@
         <v>9</v>
       </c>
       <c r="L43" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>1</v>
       </c>
       <c r="M43" s="2">
@@ -2676,7 +2816,7 @@
         <v>6</v>
       </c>
       <c r="O43" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.75065616797900259</v>
       </c>
     </row>
@@ -2688,7 +2828,7 @@
         <v>6</v>
       </c>
       <c r="C44" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.44376899696048633</v>
       </c>
       <c r="D44" s="2">
@@ -2698,7 +2838,7 @@
         <v>7</v>
       </c>
       <c r="F44" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.84259259259259267</v>
       </c>
       <c r="G44" s="2">
@@ -2708,7 +2848,7 @@
         <v>4</v>
       </c>
       <c r="I44" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.97409326424870468</v>
       </c>
       <c r="J44" s="2">
@@ -2718,7 +2858,7 @@
         <v>5</v>
       </c>
       <c r="L44" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.99250535331905776</v>
       </c>
       <c r="M44" s="2">
@@ -2728,7 +2868,7 @@
         <v>8</v>
       </c>
       <c r="O44" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.75065616797900259</v>
       </c>
     </row>
@@ -2740,7 +2880,7 @@
         <v>1</v>
       </c>
       <c r="C45" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.44376899696048633</v>
       </c>
       <c r="D45" s="2">
@@ -2750,7 +2890,7 @@
         <v>8</v>
       </c>
       <c r="F45" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.83333333333333337</v>
       </c>
       <c r="G45" s="2">
@@ -2760,7 +2900,7 @@
         <v>5</v>
       </c>
       <c r="I45" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.97020725388601037</v>
       </c>
       <c r="J45" s="2">
@@ -2770,7 +2910,7 @@
         <v>3</v>
       </c>
       <c r="L45" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.99143468950749469</v>
       </c>
       <c r="M45" s="2">
@@ -2780,7 +2920,7 @@
         <v>3</v>
       </c>
       <c r="O45" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.7165354330708662</v>
       </c>
     </row>
@@ -2792,7 +2932,7 @@
         <v>2</v>
       </c>
       <c r="C46" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.44376899696048633</v>
       </c>
       <c r="D46" s="2">
@@ -2802,7 +2942,7 @@
         <v>9</v>
       </c>
       <c r="F46" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.78703703703703698</v>
       </c>
       <c r="G46" s="2">
@@ -2812,7 +2952,7 @@
         <v>3</v>
       </c>
       <c r="I46" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.94430051813471494</v>
       </c>
       <c r="J46" s="2">
@@ -2822,7 +2962,7 @@
         <v>4</v>
       </c>
       <c r="L46" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.98822269807280516</v>
       </c>
       <c r="M46" s="2">
@@ -2832,7 +2972,7 @@
         <v>2</v>
       </c>
       <c r="O46" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.7165354330708662</v>
       </c>
     </row>
@@ -2844,7 +2984,7 @@
         <v>4</v>
       </c>
       <c r="C47" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.44376899696048633</v>
       </c>
       <c r="D47" s="2">
@@ -2854,7 +2994,7 @@
         <v>6</v>
       </c>
       <c r="F47" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.76234567901234562</v>
       </c>
       <c r="G47" s="2">
@@ -2864,7 +3004,7 @@
         <v>1</v>
       </c>
       <c r="I47" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.93393782383419688</v>
       </c>
       <c r="J47" s="2">
@@ -2874,7 +3014,7 @@
         <v>2</v>
       </c>
       <c r="L47" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.97002141327623126</v>
       </c>
       <c r="M47" s="2">
@@ -2884,7 +3024,7 @@
         <v>5</v>
       </c>
       <c r="O47" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.65616797900262469</v>
       </c>
     </row>
@@ -2896,7 +3036,7 @@
         <v>5</v>
       </c>
       <c r="C48" s="2">
-        <f t="shared" si="11"/>
+        <f t="shared" si="12"/>
         <v>0.44376899696048633</v>
       </c>
       <c r="D48" s="2">
@@ -2906,7 +3046,7 @@
         <v>5</v>
       </c>
       <c r="F48" s="2">
-        <f t="shared" si="12"/>
+        <f t="shared" si="13"/>
         <v>0.75308641975308643</v>
       </c>
       <c r="G48" s="2">
@@ -2916,7 +3056,7 @@
         <v>2</v>
       </c>
       <c r="I48" s="2">
-        <f t="shared" si="13"/>
+        <f t="shared" si="14"/>
         <v>0.87176165803108807</v>
       </c>
       <c r="J48" s="2">
@@ -2926,7 +3066,7 @@
         <v>1</v>
       </c>
       <c r="L48" s="2">
-        <f t="shared" si="14"/>
+        <f t="shared" si="15"/>
         <v>0.96145610278372584</v>
       </c>
       <c r="M48" s="2">
@@ -2936,7 +3076,7 @@
         <v>1</v>
       </c>
       <c r="O48" s="2">
-        <f t="shared" si="15"/>
+        <f t="shared" si="16"/>
         <v>0.58267716535433067</v>
       </c>
     </row>
@@ -3012,7 +3152,7 @@
         <v>1</v>
       </c>
       <c r="C51" s="2">
-        <f t="shared" ref="C51:C59" si="16">A51/$A$51</f>
+        <f t="shared" ref="C51:C59" si="17">A51/$A$51</f>
         <v>1</v>
       </c>
       <c r="D51" s="2">
@@ -3064,7 +3204,7 @@
         <v>5</v>
       </c>
       <c r="C52" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.9923518164435946</v>
       </c>
       <c r="D52" s="2">
@@ -3074,7 +3214,7 @@
         <v>7</v>
       </c>
       <c r="F52" s="2">
-        <f t="shared" ref="F52:F59" si="17">D52/$D$51</f>
+        <f t="shared" ref="F52:F59" si="18">D52/$D$51</f>
         <v>0.85585585585585588</v>
       </c>
       <c r="G52" s="2">
@@ -3084,7 +3224,7 @@
         <v>2</v>
       </c>
       <c r="I52" s="2">
-        <f t="shared" ref="I52:I59" si="18">G52/$G$51</f>
+        <f t="shared" ref="I52:I59" si="19">G52/$G$51</f>
         <v>0.97637795275590544</v>
       </c>
       <c r="J52" s="2">
@@ -3094,7 +3234,7 @@
         <v>9</v>
       </c>
       <c r="L52" s="2">
-        <f t="shared" ref="L52:L59" si="19">J52/$J$51</f>
+        <f t="shared" ref="L52:L59" si="20">J52/$J$51</f>
         <v>0.99141630901287547</v>
       </c>
       <c r="M52" s="2">
@@ -3104,7 +3244,7 @@
         <v>9</v>
       </c>
       <c r="O52" s="2">
-        <f t="shared" ref="O52:O59" si="20">M52/$M$51</f>
+        <f t="shared" ref="O52:O59" si="21">M52/$M$51</f>
         <v>0.99885844748858443</v>
       </c>
     </row>
@@ -3116,7 +3256,7 @@
         <v>4</v>
       </c>
       <c r="C53" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.9751434034416826</v>
       </c>
       <c r="D53" s="2">
@@ -3126,7 +3266,7 @@
         <v>8</v>
       </c>
       <c r="F53" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.81981981981981977</v>
       </c>
       <c r="G53" s="2">
@@ -3136,7 +3276,7 @@
         <v>1</v>
       </c>
       <c r="I53" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.93700787401574792</v>
       </c>
       <c r="J53" s="2">
@@ -3146,7 +3286,7 @@
         <v>5</v>
       </c>
       <c r="L53" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.97424892703862653</v>
       </c>
       <c r="M53" s="2">
@@ -3156,7 +3296,7 @@
         <v>7</v>
       </c>
       <c r="O53" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.99771689497716898</v>
       </c>
     </row>
@@ -3168,7 +3308,7 @@
         <v>7</v>
       </c>
       <c r="C54" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.96558317399617588</v>
       </c>
       <c r="D54" s="2">
@@ -3178,7 +3318,7 @@
         <v>5</v>
       </c>
       <c r="F54" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.78378378378378377</v>
       </c>
       <c r="G54" s="2">
@@ -3188,7 +3328,7 @@
         <v>5</v>
       </c>
       <c r="I54" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.69028871391076119</v>
       </c>
       <c r="J54" s="2">
@@ -3198,7 +3338,7 @@
         <v>4</v>
       </c>
       <c r="L54" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.94420600858369097</v>
       </c>
       <c r="M54" s="2">
@@ -3208,7 +3348,7 @@
         <v>8</v>
       </c>
       <c r="O54" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.99543378995433784</v>
       </c>
     </row>
@@ -3220,7 +3360,7 @@
         <v>6</v>
       </c>
       <c r="C55" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.92734225621414912</v>
       </c>
       <c r="D55" s="2">
@@ -3230,7 +3370,7 @@
         <v>6</v>
       </c>
       <c r="F55" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.78378378378378377</v>
       </c>
       <c r="G55" s="2">
@@ -3240,7 +3380,7 @@
         <v>6</v>
       </c>
       <c r="I55" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.68110236220472442</v>
       </c>
       <c r="J55" s="2">
@@ -3250,7 +3390,7 @@
         <v>1</v>
       </c>
       <c r="L55" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.91630901287553645</v>
       </c>
       <c r="M55" s="2">
@@ -3260,7 +3400,7 @@
         <v>5</v>
       </c>
       <c r="O55" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.97488584474885842</v>
       </c>
     </row>
@@ -3272,7 +3412,7 @@
         <v>8</v>
       </c>
       <c r="C56" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.91969407265774372</v>
       </c>
       <c r="D56" s="2">
@@ -3282,7 +3422,7 @@
         <v>3</v>
       </c>
       <c r="F56" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.72072072072072069</v>
       </c>
       <c r="G56" s="2">
@@ -3292,7 +3432,7 @@
         <v>8</v>
       </c>
       <c r="I56" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.67454068241469822</v>
       </c>
       <c r="J56" s="2">
@@ -3302,7 +3442,7 @@
         <v>7</v>
       </c>
       <c r="L56" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.91201716738197414</v>
       </c>
       <c r="M56" s="2">
@@ -3312,7 +3452,7 @@
         <v>4</v>
       </c>
       <c r="O56" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.95091324200913241</v>
       </c>
     </row>
@@ -3324,7 +3464,7 @@
         <v>9</v>
       </c>
       <c r="C57" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.910133843212237</v>
       </c>
       <c r="D57" s="2">
@@ -3334,7 +3474,7 @@
         <v>2</v>
       </c>
       <c r="F57" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.72072072072072069</v>
       </c>
       <c r="G57" s="2">
@@ -3344,7 +3484,7 @@
         <v>4</v>
       </c>
       <c r="I57" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.66535433070866146</v>
       </c>
       <c r="J57" s="2">
@@ -3354,7 +3494,7 @@
         <v>2</v>
       </c>
       <c r="L57" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.91201716738197414</v>
       </c>
       <c r="M57" s="2">
@@ -3364,7 +3504,7 @@
         <v>3</v>
       </c>
       <c r="O57" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.93835616438356162</v>
       </c>
     </row>
@@ -3376,7 +3516,7 @@
         <v>3</v>
       </c>
       <c r="C58" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.84894837476099427</v>
       </c>
       <c r="D58" s="2">
@@ -3386,7 +3526,7 @@
         <v>4</v>
       </c>
       <c r="F58" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.72072072072072069</v>
       </c>
       <c r="G58" s="2">
@@ -3396,7 +3536,7 @@
         <v>7</v>
       </c>
       <c r="I58" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.66535433070866146</v>
       </c>
       <c r="J58" s="2">
@@ -3406,7 +3546,7 @@
         <v>8</v>
       </c>
       <c r="L58" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.86909871244635195</v>
       </c>
       <c r="M58" s="2">
@@ -3416,7 +3556,7 @@
         <v>1</v>
       </c>
       <c r="O58" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.93607305936073049</v>
       </c>
     </row>
@@ -3428,7 +3568,7 @@
         <v>2</v>
       </c>
       <c r="C59" s="2">
-        <f t="shared" si="16"/>
+        <f t="shared" si="17"/>
         <v>0.8107074569789674</v>
       </c>
       <c r="D59" s="2">
@@ -3438,7 +3578,7 @@
         <v>9</v>
       </c>
       <c r="F59" s="2">
-        <f t="shared" si="17"/>
+        <f t="shared" si="18"/>
         <v>0.40990990990990989</v>
       </c>
       <c r="G59" s="2">
@@ -3448,7 +3588,7 @@
         <v>9</v>
       </c>
       <c r="I59" s="2">
-        <f t="shared" si="18"/>
+        <f t="shared" si="19"/>
         <v>0.65616797900262469</v>
       </c>
       <c r="J59" s="2">
@@ -3458,7 +3598,7 @@
         <v>3</v>
       </c>
       <c r="L59" s="2">
-        <f t="shared" si="19"/>
+        <f t="shared" si="20"/>
         <v>0.81974248927038629</v>
       </c>
       <c r="M59" s="2">
@@ -3468,7 +3608,7 @@
         <v>2</v>
       </c>
       <c r="O59" s="2">
-        <f t="shared" si="20"/>
+        <f t="shared" si="21"/>
         <v>0.92694063926940651</v>
       </c>
     </row>
@@ -3476,6 +3616,9 @@
       <c r="A62" t="s">
         <v>15</v>
       </c>
+      <c r="I62" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="63" spans="1:15">
       <c r="A63">
@@ -3485,11 +3628,18 @@
         <v>0.82312950888468905</v>
       </c>
       <c r="C63">
-        <v>1014.2</v>
+        <v>1014</v>
       </c>
       <c r="D63">
         <f>C63/$C$69</f>
-        <v>0.93440206375529755</v>
+        <v>0.93456221198156686</v>
+      </c>
+      <c r="I63">
+        <v>0.86199999999999999</v>
+      </c>
+      <c r="J63">
+        <f>I64-I63</f>
+        <v>-2.8000000000000025E-2</v>
       </c>
     </row>
     <row r="64" spans="1:15">
@@ -3500,14 +3650,21 @@
         <v>0.83256831839783252</v>
       </c>
       <c r="C64">
-        <v>1037.4000000000001</v>
+        <v>1037</v>
       </c>
       <c r="D64">
-        <f t="shared" ref="D64:D71" si="21">C64/$C$69</f>
-        <v>0.95577667219458262</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4">
+        <f t="shared" ref="D64:D71" si="22">C64/$C$69</f>
+        <v>0.95576036866359448</v>
+      </c>
+      <c r="I64">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="J64">
+        <f t="shared" ref="J64:J71" si="23">I65-I64</f>
+        <v>4.0000000000000036E-3</v>
+      </c>
+    </row>
+    <row r="65" spans="1:10">
       <c r="A65">
         <v>4</v>
       </c>
@@ -3515,14 +3672,21 @@
         <v>0.83420911784038998</v>
       </c>
       <c r="C65">
-        <v>969.7</v>
+        <v>970</v>
       </c>
       <c r="D65">
-        <f t="shared" si="21"/>
-        <v>0.89340335360235856</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4">
+        <f t="shared" si="22"/>
+        <v>0.89400921658986177</v>
+      </c>
+      <c r="I65">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="J65">
+        <f t="shared" si="23"/>
+        <v>-4.0000000000000036E-3</v>
+      </c>
+    </row>
+    <row r="66" spans="1:10">
       <c r="A66">
         <v>2</v>
       </c>
@@ -3530,14 +3694,21 @@
         <v>0.83488514384456458</v>
       </c>
       <c r="C66">
-        <v>747.7</v>
+        <v>748</v>
       </c>
       <c r="D66">
-        <f t="shared" si="21"/>
-        <v>0.68887046250230333</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4">
+        <f t="shared" si="22"/>
+        <v>0.68940092165898614</v>
+      </c>
+      <c r="I66">
+        <v>0.83399999999999996</v>
+      </c>
+      <c r="J66">
+        <f t="shared" si="23"/>
+        <v>-1.100000000000001E-2</v>
+      </c>
+    </row>
+    <row r="67" spans="1:10">
       <c r="A67">
         <v>3</v>
       </c>
@@ -3545,14 +3716,21 @@
         <v>0.83867515873420795</v>
       </c>
       <c r="C67">
-        <v>875.7</v>
+        <v>876</v>
       </c>
       <c r="D67">
-        <f t="shared" si="21"/>
-        <v>0.80679933665008285</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4">
+        <f t="shared" si="22"/>
+        <v>0.80737327188940089</v>
+      </c>
+      <c r="I67">
+        <v>0.82299999999999995</v>
+      </c>
+      <c r="J67">
+        <f t="shared" si="23"/>
+        <v>9.000000000000008E-3</v>
+      </c>
+    </row>
+    <row r="68" spans="1:10">
       <c r="A68">
         <v>1</v>
       </c>
@@ -3560,14 +3738,21 @@
         <v>0.86278967018514208</v>
       </c>
       <c r="C68">
-        <v>600.9</v>
+        <v>601</v>
       </c>
       <c r="D68">
-        <f t="shared" si="21"/>
-        <v>0.55362078496406852</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4">
+        <f>C68/$C$69</f>
+        <v>0.55391705069124419</v>
+      </c>
+      <c r="I68">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="J68">
+        <f t="shared" si="23"/>
+        <v>6.6000000000000059E-2</v>
+      </c>
+    </row>
+    <row r="69" spans="1:10">
       <c r="A69">
         <v>9</v>
       </c>
@@ -3575,14 +3760,21 @@
         <v>0.87379794842124914</v>
       </c>
       <c r="C69">
-        <v>1085.4000000000001</v>
+        <v>1085</v>
       </c>
       <c r="D69">
-        <f t="shared" si="21"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4">
+        <f t="shared" si="22"/>
+        <v>1</v>
+      </c>
+      <c r="I69">
+        <v>0.89800000000000002</v>
+      </c>
+      <c r="J69">
+        <f t="shared" si="23"/>
+        <v>-1.3000000000000012E-2</v>
+      </c>
+    </row>
+    <row r="70" spans="1:10">
       <c r="A70">
         <v>8</v>
       </c>
@@ -3590,14 +3782,21 @@
         <v>0.88586905682425932</v>
       </c>
       <c r="C70">
-        <v>1071.2</v>
+        <v>1071</v>
       </c>
       <c r="D70">
-        <f t="shared" si="21"/>
-        <v>0.98691726552423065</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4">
+        <f t="shared" si="22"/>
+        <v>0.98709677419354835</v>
+      </c>
+      <c r="I70">
+        <v>0.88500000000000001</v>
+      </c>
+      <c r="J70">
+        <f t="shared" si="23"/>
+        <v>-1.2000000000000011E-2</v>
+      </c>
+    </row>
+    <row r="71" spans="1:10">
       <c r="A71">
         <v>7</v>
       </c>
@@ -3605,11 +3804,18 @@
         <v>0.89897761834914314</v>
       </c>
       <c r="C71">
-        <v>1055.2</v>
+        <v>1055</v>
       </c>
       <c r="D71">
-        <f t="shared" si="21"/>
-        <v>0.97217615625575826</v>
+        <f t="shared" si="22"/>
+        <v>0.97235023041474655</v>
+      </c>
+      <c r="I71">
+        <v>0.873</v>
+      </c>
+      <c r="J71">
+        <f t="shared" si="23"/>
+        <v>-0.873</v>
       </c>
     </row>
   </sheetData>
@@ -3630,8 +3836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" workbookViewId="0">
-      <selection activeCell="G48" sqref="G48"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B63" sqref="B63:B71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -5834,7 +6040,7 @@
         <v>1</v>
       </c>
       <c r="B63">
-        <v>600.9</v>
+        <v>601</v>
       </c>
     </row>
     <row r="64" spans="1:15">
@@ -5842,7 +6048,7 @@
         <v>2</v>
       </c>
       <c r="B64">
-        <v>747.7</v>
+        <v>748</v>
       </c>
     </row>
     <row r="65" spans="1:2">
@@ -5850,7 +6056,7 @@
         <v>3</v>
       </c>
       <c r="B65">
-        <v>875.7</v>
+        <v>876</v>
       </c>
     </row>
     <row r="66" spans="1:2">
@@ -5858,7 +6064,7 @@
         <v>4</v>
       </c>
       <c r="B66">
-        <v>969.7</v>
+        <v>970</v>
       </c>
     </row>
     <row r="67" spans="1:2">
@@ -5866,7 +6072,7 @@
         <v>5</v>
       </c>
       <c r="B67">
-        <v>1014.2</v>
+        <v>1014</v>
       </c>
     </row>
     <row r="68" spans="1:2">
@@ -5874,7 +6080,7 @@
         <v>6</v>
       </c>
       <c r="B68">
-        <v>1037.4000000000001</v>
+        <v>1037</v>
       </c>
     </row>
     <row r="69" spans="1:2">
@@ -5882,7 +6088,7 @@
         <v>7</v>
       </c>
       <c r="B69">
-        <v>1055.2</v>
+        <v>1055</v>
       </c>
     </row>
     <row r="70" spans="1:2">
@@ -5890,7 +6096,7 @@
         <v>8</v>
       </c>
       <c r="B70">
-        <v>1071.2</v>
+        <v>1071</v>
       </c>
     </row>
     <row r="71" spans="1:2">
@@ -5898,7 +6104,7 @@
         <v>9</v>
       </c>
       <c r="B71">
-        <v>1085.4000000000001</v>
+        <v>1085</v>
       </c>
     </row>
   </sheetData>
@@ -5919,7 +6125,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView topLeftCell="A12" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
create new ranking of most common words
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="45880" yWindow="2400" windowWidth="25600" windowHeight="19020" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="22600" tabRatio="500" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="whole_word_P_R_F1" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="compare_iteration_comments" sheetId="2" r:id="rId3"/>
     <sheet name="performance of the t datasets" sheetId="4" r:id="rId4"/>
     <sheet name="compare baselines" sheetId="5" r:id="rId5"/>
+    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -23,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="256">
   <si>
     <t>design</t>
   </si>
@@ -113,6 +114,684 @@
   </si>
   <si>
     <t>delta requirement</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                5.3898</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          5.0811</t>
+  </si>
+  <si>
+    <t>(1-SW-yuck!,DESIGN)                                               4.8035</t>
+  </si>
+  <si>
+    <t>(1-SW-columns??,DESIGN)                                           4.6066</t>
+  </si>
+  <si>
+    <t>(1-SW-end-kludge,DESIGN)                                          4.5760</t>
+  </si>
+  <si>
+    <t>(1-SW-stupidity,DESIGN)                                           4.5760</t>
+  </si>
+  <si>
+    <t>(1-SW-needed?,DESIGN)                                             4.5695</t>
+  </si>
+  <si>
+    <t>(1-SW-unused?,DESIGN)                                             4.5665</t>
+  </si>
+  <si>
+    <t>(1-SW-ick!,DESIGN)                                                4.0626</t>
+  </si>
+  <si>
+    <t>(1-SW-wtf?,DESIGN)                                                4.0626</t>
+  </si>
+  <si>
+    <t>(1-SW-yuck!,DESIGN)                                               5.2466</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                5.1259</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          5.0556</t>
+  </si>
+  <si>
+    <t>(1-SW-stupidity,DESIGN)                                           5.0234</t>
+  </si>
+  <si>
+    <t>(1-SW-end-kludge,DESIGN)                                          5.0234</t>
+  </si>
+  <si>
+    <t>(1-SW-needed?,DESIGN)                                             5.0178</t>
+  </si>
+  <si>
+    <t>(1-SW-unused?,DESIGN)                                             5.0095</t>
+  </si>
+  <si>
+    <t>(1-SW-columns??,DESIGN)                                           4.7038</t>
+  </si>
+  <si>
+    <t>(1-SW-wtf?,DESIGN)                                                4.4932</t>
+  </si>
+  <si>
+    <t>(1-SW-ick!,DESIGN)</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                5.4025</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          5.0694</t>
+  </si>
+  <si>
+    <t>(1-SW-yuck!,DESIGN)                                               4.8897</t>
+  </si>
+  <si>
+    <t>(1-SW-columns??,DESIGN)                                           4.8673</t>
+  </si>
+  <si>
+    <t>(1-SW-end-kludge,DESIGN)                                          4.6694</t>
+  </si>
+  <si>
+    <t>(1-SW-stupidity,DESIGN)                                           4.6694</t>
+  </si>
+  <si>
+    <t>(1-SW-unused?,DESIGN)                                             4.6694</t>
+  </si>
+  <si>
+    <t>(1-SW-wtf?,DESIGN)                                                4.1306</t>
+  </si>
+  <si>
+    <t>(1-SW-ick!,DESIGN)                                                4.1306</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,DESIGN)                                                3.8461</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                5.4176</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          5.0496</t>
+  </si>
+  <si>
+    <t>(1-SW-yuck!,DESIGN)                                               4.7140</t>
+  </si>
+  <si>
+    <t>(1-SW-stupidity,DESIGN)                                           4.4760</t>
+  </si>
+  <si>
+    <t>(1-SW-end-kludge,DESIGN)                                          4.4760</t>
+  </si>
+  <si>
+    <t>(1-SW-needed?,DESIGN)                                             4.4741</t>
+  </si>
+  <si>
+    <t>(1-SW-unused?,DESIGN)                                             4.4722</t>
+  </si>
+  <si>
+    <t>(1-SW-ick!,DESIGN)                                                4.0071</t>
+  </si>
+  <si>
+    <t>(1-SW-wtf?,DESIGN)                                                4.0071</t>
+  </si>
+  <si>
+    <t>(1-SW-columns??,DESIGN)                                           3.9676</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                6.0130</t>
+  </si>
+  <si>
+    <t>(1-SW-yuck!,DESIGN)                                               4.9636</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          4.9382</t>
+  </si>
+  <si>
+    <t>(1-SW-end-kludge,DESIGN)                                          4.7567</t>
+  </si>
+  <si>
+    <t>(1-SW-needed?,DESIGN)                                             4.7475</t>
+  </si>
+  <si>
+    <t>(1-SW-unused?,DESIGN)                                             4.7431</t>
+  </si>
+  <si>
+    <t>(1-SW-columns??,DESIGN)                                           4.5565</t>
+  </si>
+  <si>
+    <t>(1-SW-ick!,DESIGN)                                                4.2229</t>
+  </si>
+  <si>
+    <t>(1-SW-??getridofthis,DESIGN)                                      4.0655</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,DESIGN)                                               3.9668</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                5.3205</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          4.9981</t>
+  </si>
+  <si>
+    <t>(1-SW-yuck!,DESIGN)                                               4.7239</t>
+  </si>
+  <si>
+    <t>(1-SW-columns??,DESIGN)                                           4.4986</t>
+  </si>
+  <si>
+    <t>(1-SW-stupidity,DESIGN)                                           4.4930</t>
+  </si>
+  <si>
+    <t>(1-SW-end-kludge,DESIGN)                                          4.4930</t>
+  </si>
+  <si>
+    <t>(1-SW-needed?,DESIGN)                                             4.4872</t>
+  </si>
+  <si>
+    <t>(1-SW-unused?,DESIGN)                                             4.4839</t>
+  </si>
+  <si>
+    <t>(1-SW-??getridofthis,DESIGN)                                      4.0321</t>
+  </si>
+  <si>
+    <t>(1-SW-ick!,DESIGN)                                                4.0162</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                5.2185</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          4.9826</t>
+  </si>
+  <si>
+    <t>(1-SW-yuck!,DESIGN)                                               4.7962</t>
+  </si>
+  <si>
+    <t>(1-SW-columns??,DESIGN)                                           4.7564</t>
+  </si>
+  <si>
+    <t>(1-SW-stupidity,DESIGN)                                           4.5834</t>
+  </si>
+  <si>
+    <t>(1-SW-end-kludge,DESIGN)                                          4.5834</t>
+  </si>
+  <si>
+    <t>(1-SW-needed?,DESIGN)                                             4.5724</t>
+  </si>
+  <si>
+    <t>(1-SW-unused?,DESIGN)                                             4.5679</t>
+  </si>
+  <si>
+    <t>(1-SW-ick!,DESIGN)                                                4.0799</t>
+  </si>
+  <si>
+    <t>(1-SW-wtf?,DESIGN)                                                4.0799</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                5.3056</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          5.0753</t>
+  </si>
+  <si>
+    <t>(1-SW-columns??,DESIGN)                                           4.7390</t>
+  </si>
+  <si>
+    <t>(1-SW-yuck!,DESIGN)                                               4.5891</t>
+  </si>
+  <si>
+    <t>(1-SW-stupidity,DESIGN)                                           4.3507</t>
+  </si>
+  <si>
+    <t>(1-SW-needed?,DESIGN)                                             4.3461</t>
+  </si>
+  <si>
+    <t>(1-SW-unused?,DESIGN)                                             4.3442</t>
+  </si>
+  <si>
+    <t>(1-SW-ick!,DESIGN)                                                3.8896</t>
+  </si>
+  <si>
+    <t>(1-SW-wtf?,DESIGN)                                                3.8896</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,DESIGN)                                               3.8048</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                5.4363</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          4.8612</t>
+  </si>
+  <si>
+    <t>(1-SW-yuck!,DESIGN)                                               4.8127</t>
+  </si>
+  <si>
+    <t>(1-SW-columns??,DESIGN)                                           4.6224</t>
+  </si>
+  <si>
+    <t>(1-SW-end-kludge,DESIGN)                                          4.5872</t>
+  </si>
+  <si>
+    <t>(1-SW-stupidity,DESIGN)                                           4.5872</t>
+  </si>
+  <si>
+    <t>(1-SW-needed?,DESIGN)                                             4.5829</t>
+  </si>
+  <si>
+    <t>(1-SW-ick!,DESIGN)                                                4.0900</t>
+  </si>
+  <si>
+    <t>(1-SW-wtf?,DESIGN)                                                4.0900</t>
+  </si>
+  <si>
+    <t>(1-SW-??getridofthis,DESIGN)                                      3.9370</t>
+  </si>
+  <si>
+    <t>(1-SW-hack,DESIGN)                                                5.3904</t>
+  </si>
+  <si>
+    <t>(1-SW-workaround,DESIGN)                                          5.1299</t>
+  </si>
+  <si>
+    <t>(1-SW-end-kludge,DESIGN)                                          4.7056</t>
+  </si>
+  <si>
+    <t>(1-SW-stupidity,DESIGN)                                           4.7056</t>
+  </si>
+  <si>
+    <t>(1-SW-needed?,DESIGN)                                             4.7035</t>
+  </si>
+  <si>
+    <t>(1-SW-unused?,DESIGN)                                             4.7022</t>
+  </si>
+  <si>
+    <t>(1-SW-wtf?,DESIGN)                                                4.2238</t>
+  </si>
+  <si>
+    <t>(1-SW-??getridofthis,DESIGN)                                      4.0361</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,DESIGN)                                               3.8966</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,DESIGN)                                                3.7306</t>
+  </si>
+  <si>
+    <t>hack</t>
+  </si>
+  <si>
+    <t>workaround</t>
+  </si>
+  <si>
+    <t>yuck!</t>
+  </si>
+  <si>
+    <t>columns?</t>
+  </si>
+  <si>
+    <t>kludge</t>
+  </si>
+  <si>
+    <t>stupidity</t>
+  </si>
+  <si>
+    <t>needed?</t>
+  </si>
+  <si>
+    <t>unused?</t>
+  </si>
+  <si>
+    <t>ick!</t>
+  </si>
+  <si>
+    <t>wtf?</t>
+  </si>
+  <si>
+    <t>todo</t>
+  </si>
+  <si>
+    <t>getridofthis</t>
+  </si>
+  <si>
+    <t>fixme</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        5.0549</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      4.5318</t>
+  </si>
+  <si>
+    <t>(1-SW-implementation.,IMPLEMENTATION)                             4.4484</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       4.4435</t>
+  </si>
+  <si>
+    <t>(1-SW-ends?,IMPLEMENTATION)                                       3.6061</t>
+  </si>
+  <si>
+    <t>(1-SW-convention,IMPLEMENTATION)                                  3.2698</t>
+  </si>
+  <si>
+    <t>(1-SW-apparently,IMPLEMENTATION)                                  2.8350</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         2.8190</t>
+  </si>
+  <si>
+    <t>(1-SW-configurable,IMPLEMENTATION)                                2.6630</t>
+  </si>
+  <si>
+    <t>(1-SW-auto-generated,IMPLEMENTATION)                              2.3603</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        5.1281</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      4.6795</t>
+  </si>
+  <si>
+    <t>(1-SW-implementation.,IMPLEMENTATION)                             4.4441</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       4.3626</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         3.5211</t>
+  </si>
+  <si>
+    <t>(1-SW-ends?,IMPLEMENTATION)                                       3.4189</t>
+  </si>
+  <si>
+    <t>(1-SW-configurable,IMPLEMENTATION)                                3.0117</t>
+  </si>
+  <si>
+    <t>(1-SW-convention,IMPLEMENTATION)                                  2.9818</t>
+  </si>
+  <si>
+    <t>(1-SW-apparently,IMPLEMENTATION)                                  2.6847</t>
+  </si>
+  <si>
+    <t>(1-SW-1st,IMPLEMENTATION)                                         2.3792</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        5.4335</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       4.2730</t>
+  </si>
+  <si>
+    <t>(1-SW-implemented,IMPLEMENTATION)                                 3.7028</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         3.4405</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      2.9431</t>
+  </si>
+  <si>
+    <t>(1-SW-configurable,IMPLEMENTATION)                                2.6160</t>
+  </si>
+  <si>
+    <t>(1-SW-convention,IMPLEMENTATION)                                  2.6073</t>
+  </si>
+  <si>
+    <t>(1-SW-handled,IMPLEMENTATION)                                     2.2022</t>
+  </si>
+  <si>
+    <t>(1-SW-tbd,IMPLEMENTATION)                                         2.0578</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        5.0784</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      4.5033</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       4.4533</t>
+  </si>
+  <si>
+    <t>(1-SW-implementation.,IMPLEMENTATION)                             4.3253</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         3.5198</t>
+  </si>
+  <si>
+    <t>(1-SW-ends?,IMPLEMENTATION)                                       3.3826</t>
+  </si>
+  <si>
+    <t>(1-SW-convention,IMPLEMENTATION)                                  3.0726</t>
+  </si>
+  <si>
+    <t>(1-SW-apparently,IMPLEMENTATION)                                  2.7577</t>
+  </si>
+  <si>
+    <t>(1-SW-configurable,IMPLEMENTATION)                                2.7275</t>
+  </si>
+  <si>
+    <t>(1-SW-tbd,IMPLEMENTATION)                                         2.4288</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        5.0625</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      4.5398</t>
+  </si>
+  <si>
+    <t>(1-SW-implementation.,IMPLEMENTATION)                             4.5129</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       4.4733</t>
+  </si>
+  <si>
+    <t>(1-SW-ends?,IMPLEMENTATION)                                       3.6415</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         3.5019</t>
+  </si>
+  <si>
+    <t>(1-SW-convention,IMPLEMENTATION)                                  3.2656</t>
+  </si>
+  <si>
+    <t>(1-SW-configurable,IMPLEMENTATION)                                2.7687</t>
+  </si>
+  <si>
+    <t>(1-SW-apparently,IMPLEMENTATION)                                  2.5963</t>
+  </si>
+  <si>
+    <t>(1-SW-auto-generated,IMPLEMENTATION)                              2.3764</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        4.8943</t>
+  </si>
+  <si>
+    <t>(1-SW-implementation.,IMPLEMENTATION)                             4.5294</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      4.5042</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       4.4158</t>
+  </si>
+  <si>
+    <t>(1-SW-ends?,IMPLEMENTATION)                                       3.4600</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         3.4401</t>
+  </si>
+  <si>
+    <t>(1-SW-convention,IMPLEMENTATION)                                  3.1417</t>
+  </si>
+  <si>
+    <t>(1-SW-apparently,IMPLEMENTATION)                                  2.7769</t>
+  </si>
+  <si>
+    <t>(1-SW-configurable,IMPLEMENTATION)                                2.7738</t>
+  </si>
+  <si>
+    <t>(1-SW-auto-generated,IMPLEMENTATION)                              2.5780</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        5.2476</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       4.6605</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      4.6091</t>
+  </si>
+  <si>
+    <t>(1-SW-implementation.,IMPLEMENTATION)                             4.5641</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         3.9060</t>
+  </si>
+  <si>
+    <t>(1-SW-ends?,IMPLEMENTATION)                                       3.4788</t>
+  </si>
+  <si>
+    <t>(1-SW-configurable,IMPLEMENTATION)                                2.9565</t>
+  </si>
+  <si>
+    <t>(1-SW-apparently,IMPLEMENTATION)                                  2.7915</t>
+  </si>
+  <si>
+    <t>(1-SW-auto-generated,IMPLEMENTATION)                              2.4790</t>
+  </si>
+  <si>
+    <t>(1-SW-1st,IMPLEMENTATION)                                         2.3592</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        5.0844</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       4.8124</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      4.5536</t>
+  </si>
+  <si>
+    <t>(1-SW-implementation.,IMPLEMENTATION)                             4.5106</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         3.4842</t>
+  </si>
+  <si>
+    <t>(1-SW-ends?,IMPLEMENTATION)                                       3.4792</t>
+  </si>
+  <si>
+    <t>(1-SW-convention,IMPLEMENTATION)                                  3.1165</t>
+  </si>
+  <si>
+    <t>(1-SW-apparently,IMPLEMENTATION)                                  2.7835</t>
+  </si>
+  <si>
+    <t>(1-SW-1st,IMPLEMENTATION)                                         2.3795</t>
+  </si>
+  <si>
+    <t>(1-SW-auto-generated,IMPLEMENTATION)                              2.3423</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        4.9109</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      4.5105</t>
+  </si>
+  <si>
+    <t>(1-SW-implementation.,IMPLEMENTATION)                             4.4735</t>
+  </si>
+  <si>
+    <t>(1-SW-ends?,IMPLEMENTATION)                                       3.5787</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       3.2142</t>
+  </si>
+  <si>
+    <t>(1-SW-convention,IMPLEMENTATION)                                  3.1658</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         3.1430</t>
+  </si>
+  <si>
+    <t>(1-SW-apparently,IMPLEMENTATION)                                  2.7570</t>
+  </si>
+  <si>
+    <t>(1-SW-configurable,IMPLEMENTATION)                                2.7461</t>
+  </si>
+  <si>
+    <t>(1-SW-todo,IMPLEMENTATION)                                        5.0246</t>
+  </si>
+  <si>
+    <t>(1-SW-implementation.,IMPLEMENTATION)                             4.4857</t>
+  </si>
+  <si>
+    <t>(1-SW-needed,IMPLEMENTATION)                                      4.3802</t>
+  </si>
+  <si>
+    <t>(1-SW-fixme,IMPLEMENTATION)                                       4.2917</t>
+  </si>
+  <si>
+    <t>(1-SW-ends?,IMPLEMENTATION)                                       3.4624</t>
+  </si>
+  <si>
+    <t>(1-SW-xxx,IMPLEMENTATION)                                         3.3457</t>
+  </si>
+  <si>
+    <t>(1-SW-convention,IMPLEMENTATION)                                  3.0746</t>
+  </si>
+  <si>
+    <t>(1-SW-configurable,IMPLEMENTATION)                                2.7086</t>
+  </si>
+  <si>
+    <t>(1-SW-apparently,IMPLEMENTATION)                                  2.6717</t>
+  </si>
+  <si>
+    <t>(1-SW-1st,IMPLEMENTATION)                                         2.2489</t>
+  </si>
+  <si>
+    <t>needed</t>
+  </si>
+  <si>
+    <t>implementation</t>
+  </si>
+  <si>
+    <t>ends?</t>
+  </si>
+  <si>
+    <t>convention</t>
+  </si>
+  <si>
+    <t>apparently</t>
+  </si>
+  <si>
+    <t>xxx</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1-SW-auto-generated,IMPLEMENTATION) </t>
+  </si>
+  <si>
+    <t>configurable</t>
+  </si>
+  <si>
+    <t>auto-generated</t>
+  </si>
+  <si>
+    <t>1st</t>
+  </si>
+  <si>
+    <t>tdb</t>
+  </si>
+  <si>
+    <t>handled</t>
+  </si>
+  <si>
+    <t>((1-SW-recursion,IMPLEMENTATION)                                   1.9013</t>
+  </si>
+  <si>
+    <t>recursion</t>
   </si>
 </sst>
 </file>
@@ -144,12 +823,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -161,7 +846,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="137">
+  <cellStyleXfs count="199">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -299,13 +984,76 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="137">
+  <cellStyles count="199">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -374,6 +1122,37 @@
     <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="154" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="156" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="158" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="160" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="162" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="164" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="166" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="168" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="170" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="172" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="174" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="176" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="178" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="180" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="182" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="184" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="186" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="188" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="190" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="192" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -442,6 +1221,37 @@
     <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="153" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="155" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="157" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="159" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="161" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="163" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="165" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="167" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="169" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="171" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="173" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="175" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="177" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="179" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="181" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="183" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="185" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="187" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="189" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="191" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -773,7 +1583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O44"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="A31" sqref="A31"/>
     </sheetView>
   </sheetViews>
@@ -1293,8 +2103,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="J63" sqref="J63:J71"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -3836,8 +4646,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O71"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="B63" sqref="B63:B71"/>
+    <sheetView topLeftCell="A11" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -6432,4 +7242,1145 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F73"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="A70" sqref="A70"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <cols>
+    <col min="1" max="1" width="19.6640625" customWidth="1"/>
+    <col min="2" max="2" width="20.33203125" customWidth="1"/>
+    <col min="3" max="3" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="24.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26.1640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="F1" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="F2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="F3" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="F4" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="F5" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="F6" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="F8" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="A9" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="F9" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F10" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
+      <c r="A11" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="F11" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
+      <c r="F12" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="F13" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
+      <c r="A14" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B14" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="C14" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="F14" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
+      <c r="A15" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="F15" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>124</v>
+      </c>
+      <c r="F16" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="D17" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="F17" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6">
+      <c r="A18" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="F18" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6">
+      <c r="A19" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="F19" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="F20" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6">
+      <c r="A21" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="C21" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="D21" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="F21" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6">
+      <c r="A22" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="F22" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6">
+      <c r="A24" t="s">
+        <v>131</v>
+      </c>
+      <c r="B24">
+        <f>1+2+1+1+1+1+1+1+1+1</f>
+        <v>11</v>
+      </c>
+      <c r="C24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6">
+      <c r="A25" t="s">
+        <v>132</v>
+      </c>
+      <c r="B25">
+        <f>2+3+2+2+3+2+3+2+2+2</f>
+        <v>23</v>
+      </c>
+      <c r="C25">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6">
+      <c r="A26" t="s">
+        <v>133</v>
+      </c>
+      <c r="B26">
+        <f>3+1+3+3+3+2+3+3+4+3+11</f>
+        <v>39</v>
+      </c>
+      <c r="C26">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6">
+      <c r="A27" t="s">
+        <v>134</v>
+      </c>
+      <c r="B27">
+        <f>4+9+4+10+7+4+4+3+4+4+11</f>
+        <v>64</v>
+      </c>
+      <c r="C27">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6">
+      <c r="A28" t="s">
+        <v>135</v>
+      </c>
+      <c r="B28">
+        <f>5+5+5+6+4+6+6+11+5+3</f>
+        <v>56</v>
+      </c>
+      <c r="C28">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6">
+      <c r="A29" t="s">
+        <v>136</v>
+      </c>
+      <c r="B29">
+        <f>6+4+6+4+11+5+5+5+6+4</f>
+        <v>56</v>
+      </c>
+      <c r="C29">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" t="s">
+        <v>137</v>
+      </c>
+      <c r="B30">
+        <f>7+6+11+6+5+7+7+6+7+D75</f>
+        <v>62</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6">
+      <c r="A31" t="s">
+        <v>138</v>
+      </c>
+      <c r="B31">
+        <f>8+7+7+7+6+8+8+7+11+6</f>
+        <v>75</v>
+      </c>
+      <c r="C31">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6">
+      <c r="A32" t="s">
+        <v>139</v>
+      </c>
+      <c r="B32">
+        <f>9+8+9+8+8+10+9+8+8+11</f>
+        <v>88</v>
+      </c>
+      <c r="C32">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6">
+      <c r="A33" t="s">
+        <v>140</v>
+      </c>
+      <c r="B33">
+        <f>10+10+8+9+11+11+10+9+9+7</f>
+        <v>94</v>
+      </c>
+      <c r="C33">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6">
+      <c r="A34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34">
+        <f>11+11+10+11+11+11+11+11+10</f>
+        <v>97</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6">
+      <c r="A35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35">
+        <f>11+11+11+11+9+9+11+11+10+8</f>
+        <v>102</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6">
+      <c r="A36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36">
+        <f>11+11+11+11+10+11+11+10+11+9</f>
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6">
+      <c r="A38" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C38" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="E38" s="3" t="s">
+        <v>183</v>
+      </c>
+      <c r="F38" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6">
+      <c r="A39" s="3" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>155</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>165</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>174</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="F39" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6">
+      <c r="A40" s="3" t="s">
+        <v>146</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="D40" s="3" t="s">
+        <v>175</v>
+      </c>
+      <c r="E40" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="F40" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6">
+      <c r="A41" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B41" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="C41" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="D41" s="3" t="s">
+        <v>176</v>
+      </c>
+      <c r="E41" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="F41" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6">
+      <c r="A42" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B42" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="D42" s="3" t="s">
+        <v>177</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>187</v>
+      </c>
+      <c r="F42" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6">
+      <c r="A43" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B43" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="C43" s="3" t="s">
+        <v>169</v>
+      </c>
+      <c r="D43" s="3" t="s">
+        <v>178</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="F43" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6">
+      <c r="A44" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B44" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="C44" s="3" t="s">
+        <v>170</v>
+      </c>
+      <c r="D44" s="3" t="s">
+        <v>179</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>189</v>
+      </c>
+      <c r="F44" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6">
+      <c r="A45" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="C45" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="D45" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>190</v>
+      </c>
+      <c r="F45" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6">
+      <c r="A46" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B46" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="D46" s="3" t="s">
+        <v>181</v>
+      </c>
+      <c r="E46" s="3" t="s">
+        <v>191</v>
+      </c>
+      <c r="F46" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6">
+      <c r="A47" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B47" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="C47" t="s">
+        <v>254</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>182</v>
+      </c>
+      <c r="E47" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="F47" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6">
+      <c r="A49" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="B49" s="3" t="s">
+        <v>203</v>
+      </c>
+      <c r="C49" s="3" t="s">
+        <v>213</v>
+      </c>
+      <c r="D49" s="3" t="s">
+        <v>223</v>
+      </c>
+      <c r="E49" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="F49" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6">
+      <c r="A50" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="B50" s="3" t="s">
+        <v>204</v>
+      </c>
+      <c r="C50" s="3" t="s">
+        <v>214</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>224</v>
+      </c>
+      <c r="E50" s="3" t="s">
+        <v>233</v>
+      </c>
+      <c r="F50" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6">
+      <c r="A51" s="3" t="s">
+        <v>195</v>
+      </c>
+      <c r="B51" s="3" t="s">
+        <v>205</v>
+      </c>
+      <c r="C51" s="3" t="s">
+        <v>215</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>225</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>234</v>
+      </c>
+      <c r="F51" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6">
+      <c r="A52" s="3" t="s">
+        <v>196</v>
+      </c>
+      <c r="B52" s="3" t="s">
+        <v>206</v>
+      </c>
+      <c r="C52" s="3" t="s">
+        <v>216</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>226</v>
+      </c>
+      <c r="E52" s="3" t="s">
+        <v>235</v>
+      </c>
+      <c r="F52" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6">
+      <c r="A53" s="3" t="s">
+        <v>197</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>207</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>217</v>
+      </c>
+      <c r="D53" s="3" t="s">
+        <v>227</v>
+      </c>
+      <c r="E53" s="3" t="s">
+        <v>236</v>
+      </c>
+      <c r="F53" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6">
+      <c r="A54" s="3" t="s">
+        <v>198</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>208</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>218</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>228</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>237</v>
+      </c>
+      <c r="F54" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6">
+      <c r="A55" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="B55" s="3" t="s">
+        <v>209</v>
+      </c>
+      <c r="C55" s="3" t="s">
+        <v>219</v>
+      </c>
+      <c r="D55" s="3" t="s">
+        <v>229</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>238</v>
+      </c>
+      <c r="F55" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6">
+      <c r="A56" s="3" t="s">
+        <v>200</v>
+      </c>
+      <c r="B56" s="3" t="s">
+        <v>210</v>
+      </c>
+      <c r="C56" s="3" t="s">
+        <v>220</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>230</v>
+      </c>
+      <c r="E56" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="F56" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6">
+      <c r="A57" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="B57" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>221</v>
+      </c>
+      <c r="D57" s="3" t="s">
+        <v>231</v>
+      </c>
+      <c r="E57" s="3" t="s">
+        <v>240</v>
+      </c>
+      <c r="F57" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6">
+      <c r="A58" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="B58" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="C58" s="3" t="s">
+        <v>222</v>
+      </c>
+      <c r="D58" s="3" t="s">
+        <v>248</v>
+      </c>
+      <c r="E58" s="3" t="s">
+        <v>241</v>
+      </c>
+      <c r="F58" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6">
+      <c r="A60" t="s">
+        <v>141</v>
+      </c>
+      <c r="B60">
+        <f>1+1+1+1+1+1+1+1+1+1</f>
+        <v>10</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6">
+      <c r="A61" t="s">
+        <v>242</v>
+      </c>
+      <c r="B61">
+        <f>2+2+5+2+2+3+3+3+2+3</f>
+        <v>27</v>
+      </c>
+      <c r="C61">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6">
+      <c r="A62" t="s">
+        <v>243</v>
+      </c>
+      <c r="B62">
+        <f>3+3+3+4+3+2+4+4+3+2</f>
+        <v>31</v>
+      </c>
+      <c r="C62">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6">
+      <c r="A63" t="s">
+        <v>143</v>
+      </c>
+      <c r="B63" s="2">
+        <f>4+4+2+3+4+4+2+2+5+4</f>
+        <v>34</v>
+      </c>
+      <c r="C63">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6">
+      <c r="A64" t="s">
+        <v>244</v>
+      </c>
+      <c r="B64">
+        <f>5+6+11+6+5+5+6+6+4+5</f>
+        <v>59</v>
+      </c>
+      <c r="C64">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3">
+      <c r="A65" t="s">
+        <v>245</v>
+      </c>
+      <c r="B65">
+        <f>6+8+7+7+7+7+11+7+6+7</f>
+        <v>73</v>
+      </c>
+      <c r="C65">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3">
+      <c r="A66" t="s">
+        <v>246</v>
+      </c>
+      <c r="B66">
+        <f>7+9+11+8+9+8+8+8+8+9</f>
+        <v>85</v>
+      </c>
+      <c r="C66">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3">
+      <c r="A67" t="s">
+        <v>247</v>
+      </c>
+      <c r="B67">
+        <f>8+5+4+5+6+6+5+5+7+6</f>
+        <v>57</v>
+      </c>
+      <c r="C67">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3">
+      <c r="A68" t="s">
+        <v>249</v>
+      </c>
+      <c r="B68">
+        <f>9+7+6+9+8+9+7+11+9+8</f>
+        <v>83</v>
+      </c>
+      <c r="C68">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3">
+      <c r="A69" t="s">
+        <v>250</v>
+      </c>
+      <c r="B69">
+        <f>10+11+11+11+10+10+9+10+10+11</f>
+        <v>103</v>
+      </c>
+      <c r="C69">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3">
+      <c r="A70" t="s">
+        <v>251</v>
+      </c>
+      <c r="B70">
+        <f>11+10+11+11+11+11+10+9+11+10</f>
+        <v>105</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3">
+      <c r="A71" t="s">
+        <v>252</v>
+      </c>
+      <c r="B71">
+        <f>11+11+9+10+11+11+11+11+11+11</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3">
+      <c r="A72" t="s">
+        <v>253</v>
+      </c>
+      <c r="B72">
+        <f>11+11+8+11+11+11+11+11+11+11</f>
+        <v>107</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3">
+      <c r="A73" t="s">
+        <v>255</v>
+      </c>
+      <c r="B73">
+        <f>11+11+10+11+11+11+11+11+11+11</f>
+        <v>109</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
collecting results for the discussion
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="22600" tabRatio="500" activeTab="5"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="22600" tabRatio="500" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="whole_word_P_R_F1" sheetId="1" r:id="rId1"/>
@@ -13,6 +13,7 @@
     <sheet name="performance of the t datasets" sheetId="4" r:id="rId4"/>
     <sheet name="compare baselines" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
+    <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="414" uniqueCount="256">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="262">
   <si>
     <t>design</t>
   </si>
@@ -792,6 +793,24 @@
   </si>
   <si>
     <t>recursion</t>
+  </si>
+  <si>
+    <t>F1 measure</t>
+  </si>
+  <si>
+    <t>Precision</t>
+  </si>
+  <si>
+    <t>Recall</t>
+  </si>
+  <si>
+    <t>LR</t>
+  </si>
+  <si>
+    <t>Binary</t>
+  </si>
+  <si>
+    <t>Bayes</t>
   </si>
 </sst>
 </file>
@@ -846,8 +865,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="199">
+  <cellStyleXfs count="215">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1053,7 +1088,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="199">
+  <cellStyles count="215">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1153,6 +1188,14 @@
     <cellStyle name="Followed Hyperlink" xfId="194" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="196" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="198" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="200" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="202" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="204" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="206" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="208" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1252,6 +1295,14 @@
     <cellStyle name="Hyperlink" xfId="193" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="195" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="197" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="199" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="201" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="203" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="205" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="207" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7248,8 +7299,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A47" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
-      <selection activeCell="A70" sqref="A70"/>
+    <sheetView topLeftCell="A33" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+      <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -8383,4 +8434,795 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G41"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetData>
+    <row r="1" spans="1:7">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" t="s">
+        <v>256</v>
+      </c>
+      <c r="E2" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" t="s">
+        <v>259</v>
+      </c>
+      <c r="B3" t="s">
+        <v>260</v>
+      </c>
+      <c r="C3" t="s">
+        <v>261</v>
+      </c>
+      <c r="E3" t="s">
+        <v>259</v>
+      </c>
+      <c r="F3" t="s">
+        <v>260</v>
+      </c>
+      <c r="G3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4">
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="B4">
+        <v>0.56299999999999994</v>
+      </c>
+      <c r="C4">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="E4">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="F4">
+        <v>0.41399999999999998</v>
+      </c>
+      <c r="G4">
+        <v>0.03</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="B5">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="C5">
+        <v>0.52500000000000002</v>
+      </c>
+      <c r="E5">
+        <v>0.255</v>
+      </c>
+      <c r="F5">
+        <v>0.76</v>
+      </c>
+      <c r="G5">
+        <v>0.33500000000000002</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6">
+        <v>0.81399999999999995</v>
+      </c>
+      <c r="B6">
+        <v>0.627</v>
+      </c>
+      <c r="C6">
+        <v>0.29399999999999998</v>
+      </c>
+      <c r="E6">
+        <v>0.76</v>
+      </c>
+      <c r="F6">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="G6">
+        <v>0.189</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7">
+        <v>0.60099999999999998</v>
+      </c>
+      <c r="B7">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="C7">
+        <v>0.106</v>
+      </c>
+      <c r="E7">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="F7">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="G7">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8">
+        <v>0.47</v>
+      </c>
+      <c r="B8">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="C8">
+        <v>0.435</v>
+      </c>
+      <c r="E8">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.48499999999999999</v>
+      </c>
+      <c r="G8">
+        <v>9.7000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9">
+        <v>0.74399999999999999</v>
+      </c>
+      <c r="B9">
+        <v>0.48</v>
+      </c>
+      <c r="C9">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="E9">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="F9">
+        <v>9.5000000000000001E-2</v>
+      </c>
+      <c r="G9">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
+      <c r="A10">
+        <v>0.50900000000000001</v>
+      </c>
+      <c r="B10">
+        <v>0.495</v>
+      </c>
+      <c r="C10">
+        <v>0.35</v>
+      </c>
+      <c r="E10">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="F10">
+        <v>0.45900000000000002</v>
+      </c>
+      <c r="G10">
+        <v>3.9E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
+      <c r="A11">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="B11">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.224</v>
+      </c>
+      <c r="E11">
+        <v>0.5</v>
+      </c>
+      <c r="F11">
+        <v>0.28599999999999998</v>
+      </c>
+      <c r="G11">
+        <v>2.9000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="A12">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="B12">
+        <v>0.81100000000000005</v>
+      </c>
+      <c r="C12">
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="E12">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="F12">
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="G12">
+        <v>0.13700000000000001</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="A13">
+        <v>0.54</v>
+      </c>
+      <c r="B13">
+        <v>0.55800000000000005</v>
+      </c>
+      <c r="C13">
+        <v>0.23300000000000001</v>
+      </c>
+      <c r="E13">
+        <v>0.875</v>
+      </c>
+      <c r="F13">
+        <v>0.82</v>
+      </c>
+      <c r="G13">
+        <v>0.121</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7">
+      <c r="A14">
+        <f>AVERAGE(A4:A13)</f>
+        <v>0.6201000000000001</v>
+      </c>
+      <c r="B14">
+        <f>AVERAGE(B4:B13)</f>
+        <v>0.63479999999999992</v>
+      </c>
+      <c r="C14">
+        <f>AVERAGE(C4:C13)</f>
+        <v>0.30830000000000002</v>
+      </c>
+      <c r="E14">
+        <f>AVERAGE(E4:E13)</f>
+        <v>0.50980000000000003</v>
+      </c>
+      <c r="F14">
+        <f>AVERAGE(F4:F13)</f>
+        <v>0.51019999999999999</v>
+      </c>
+      <c r="G14">
+        <f>AVERAGE(G4:G13)</f>
+        <v>0.10170000000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7">
+      <c r="A16" t="s">
+        <v>257</v>
+      </c>
+      <c r="E16" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
+      <c r="A17" t="s">
+        <v>259</v>
+      </c>
+      <c r="B17" t="s">
+        <v>260</v>
+      </c>
+      <c r="C17" t="s">
+        <v>261</v>
+      </c>
+      <c r="E17" t="s">
+        <v>259</v>
+      </c>
+      <c r="F17" t="s">
+        <v>260</v>
+      </c>
+      <c r="G17" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
+      <c r="A18">
+        <v>0.55400000000000005</v>
+      </c>
+      <c r="B18">
+        <v>0.62</v>
+      </c>
+      <c r="C18">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="E18">
+        <v>0.35299999999999998</v>
+      </c>
+      <c r="F18">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="G18">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
+      <c r="A19">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="B19">
+        <v>0.79</v>
+      </c>
+      <c r="C19">
+        <v>0.35799999999999998</v>
+      </c>
+      <c r="E19">
+        <v>0.16700000000000001</v>
+      </c>
+      <c r="F19">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="G19">
+        <v>0.20699999999999999</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
+      <c r="A20">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="B20">
+        <v>0.84</v>
+      </c>
+      <c r="C20">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="E20">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="F20">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="G20">
+        <v>0.105</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
+      <c r="A21">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="B21">
+        <v>0.63300000000000001</v>
+      </c>
+      <c r="C21">
+        <v>5.7000000000000002E-2</v>
+      </c>
+      <c r="E21">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="F21">
+        <v>0.8</v>
+      </c>
+      <c r="G21">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
+      <c r="A22">
+        <v>0.57399999999999995</v>
+      </c>
+      <c r="B22">
+        <v>0.89500000000000002</v>
+      </c>
+      <c r="C22">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="E22">
+        <v>0.8</v>
+      </c>
+      <c r="F22">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="G22">
+        <v>5.0999999999999997E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
+      <c r="A23">
+        <v>0.877</v>
+      </c>
+      <c r="B23">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="C23">
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="E23">
+        <v>0.61</v>
+      </c>
+      <c r="F23">
+        <v>0.14299999999999999</v>
+      </c>
+      <c r="G23">
+        <v>0.01</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7">
+      <c r="A24">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="B24">
+        <v>0.65800000000000003</v>
+      </c>
+      <c r="C24">
+        <v>0.224</v>
+      </c>
+      <c r="E24">
+        <v>0.125</v>
+      </c>
+      <c r="F24">
+        <v>0.34699999999999998</v>
+      </c>
+      <c r="G24">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7">
+      <c r="A25">
+        <v>0.64600000000000002</v>
+      </c>
+      <c r="B25">
+        <v>0.81899999999999995</v>
+      </c>
+      <c r="C25">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="E25">
+        <v>0.373</v>
+      </c>
+      <c r="F25">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G25">
+        <v>1.4999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7">
+      <c r="A26">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="B26">
+        <v>0.81499999999999995</v>
+      </c>
+      <c r="C26">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="E26">
+        <v>0.70899999999999996</v>
+      </c>
+      <c r="F26">
+        <v>0.70199999999999996</v>
+      </c>
+      <c r="G26">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27">
+        <v>0.54400000000000004</v>
+      </c>
+      <c r="B27">
+        <v>0.56699999999999995</v>
+      </c>
+      <c r="C27">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="E27">
+        <v>0.91300000000000003</v>
+      </c>
+      <c r="F27">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="G27">
+        <v>6.4000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7">
+      <c r="A28">
+        <f>AVERAGE(A18:A27)</f>
+        <v>0.71599999999999997</v>
+      </c>
+      <c r="B28">
+        <f>AVERAGE(B18:B27)</f>
+        <v>0.74440000000000006</v>
+      </c>
+      <c r="C28">
+        <f>AVERAGE(C18:C27)</f>
+        <v>0.19550000000000001</v>
+      </c>
+      <c r="E28">
+        <f>AVERAGE(E18:E27)</f>
+        <v>0.5766</v>
+      </c>
+      <c r="F28">
+        <f>AVERAGE(F18:F27)</f>
+        <v>0.58010000000000006</v>
+      </c>
+      <c r="G28">
+        <f>AVERAGE(G18:G27)</f>
+        <v>5.7099999999999998E-2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7">
+      <c r="A29" t="s">
+        <v>258</v>
+      </c>
+      <c r="E29" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
+      <c r="A30" t="s">
+        <v>259</v>
+      </c>
+      <c r="B30" t="s">
+        <v>260</v>
+      </c>
+      <c r="C30" t="s">
+        <v>261</v>
+      </c>
+      <c r="E30" t="s">
+        <v>259</v>
+      </c>
+      <c r="F30" t="s">
+        <v>260</v>
+      </c>
+      <c r="G30" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7">
+      <c r="A31">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="B31">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="C31">
+        <v>0.874</v>
+      </c>
+      <c r="E31">
+        <v>0.375</v>
+      </c>
+      <c r="F31">
+        <v>0.375</v>
+      </c>
+      <c r="G31">
+        <v>0.86799999999999999</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7">
+      <c r="A32">
+        <v>0.66800000000000004</v>
+      </c>
+      <c r="B32">
+        <v>0.85799999999999998</v>
+      </c>
+      <c r="C32">
+        <v>0.98499999999999999</v>
+      </c>
+      <c r="E32">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="F32">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="G32">
+        <v>0.877</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7">
+      <c r="A33">
+        <v>0.84299999999999997</v>
+      </c>
+      <c r="B33">
+        <v>0.5</v>
+      </c>
+      <c r="C33">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="E33">
+        <v>0.72199999999999998</v>
+      </c>
+      <c r="F33">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="G33">
+        <v>0.97799999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="B34">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="C34">
+        <v>0.872</v>
+      </c>
+      <c r="E34">
+        <v>0.95499999999999996</v>
+      </c>
+      <c r="F34">
+        <v>0.25</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="A35">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="B35">
+        <v>0.67</v>
+      </c>
+      <c r="C35">
+        <v>0.89</v>
+      </c>
+      <c r="E35">
+        <v>0.25</v>
+      </c>
+      <c r="F35">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="G35">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="A36">
+        <v>0.64500000000000002</v>
+      </c>
+      <c r="B36">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="C36">
+        <v>0.79100000000000004</v>
+      </c>
+      <c r="E36">
+        <v>0.39100000000000001</v>
+      </c>
+      <c r="F36">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="G36">
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7">
+      <c r="A37">
+        <v>0.378</v>
+      </c>
+      <c r="B37">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="C37">
+        <v>0.80100000000000005</v>
+      </c>
+      <c r="E37">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="F37">
+        <v>0.68</v>
+      </c>
+      <c r="G37">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7">
+      <c r="A38">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="B38">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="C38">
+        <v>0.56000000000000005</v>
+      </c>
+      <c r="E38">
+        <v>0.76</v>
+      </c>
+      <c r="F38">
+        <v>0.54500000000000004</v>
+      </c>
+      <c r="G38">
+        <v>0.95499999999999996</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7">
+      <c r="A39">
+        <v>0.77</v>
+      </c>
+      <c r="B39">
+        <v>0.80800000000000005</v>
+      </c>
+      <c r="C39">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="E39">
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="F39">
+        <v>0.35099999999999998</v>
+      </c>
+      <c r="G39">
+        <v>0.90400000000000003</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7">
+      <c r="A40">
+        <v>0.53600000000000003</v>
+      </c>
+      <c r="B40">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="C40">
+        <v>0.94699999999999995</v>
+      </c>
+      <c r="E40">
+        <v>0.84</v>
+      </c>
+      <c r="F40">
+        <v>0.83299999999999996</v>
+      </c>
+      <c r="G40">
+        <v>0.96699999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7">
+      <c r="A41">
+        <f>AVERAGE(A31:A40)</f>
+        <v>0.56020000000000003</v>
+      </c>
+      <c r="B41">
+        <f>AVERAGE(B31:B40)</f>
+        <v>0.57089999999999996</v>
+      </c>
+      <c r="C41">
+        <f>AVERAGE(C31:C40)</f>
+        <v>0.84770000000000001</v>
+      </c>
+      <c r="E41">
+        <f>AVERAGE(E31:E40)</f>
+        <v>0.5250999999999999</v>
+      </c>
+      <c r="F41">
+        <f>AVERAGE(F31:F40)</f>
+        <v>0.51819999999999999</v>
+      </c>
+      <c r="G41">
+        <f>AVERAGE(G31:G40)</f>
+        <v>0.90190000000000003</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add figures and complement missing discussion
</commit_message>
<xml_diff>
--- a/averages.xlsx
+++ b/averages.xlsx
@@ -4,16 +4,16 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26221"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="22600" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="38400" yWindow="0" windowWidth="38400" windowHeight="22600" tabRatio="500" firstSheet="1" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="whole_word_P_R_F1" sheetId="1" r:id="rId1"/>
     <sheet name="compare_iteration_F1" sheetId="3" r:id="rId2"/>
     <sheet name="compare_iteration_comments" sheetId="2" r:id="rId3"/>
     <sheet name="performance of the t datasets" sheetId="4" r:id="rId4"/>
-    <sheet name="compare baselines" sheetId="5" r:id="rId5"/>
-    <sheet name="Sheet1" sheetId="6" r:id="rId6"/>
-    <sheet name="Sheet2" sheetId="7" r:id="rId7"/>
+    <sheet name="improviment over baseline" sheetId="5" r:id="rId5"/>
+    <sheet name="ranking words" sheetId="6" r:id="rId6"/>
+    <sheet name="algorithms performance" sheetId="7" r:id="rId7"/>
   </sheets>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="440" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="263">
   <si>
     <t>design</t>
   </si>
@@ -811,6 +811,9 @@
   </si>
   <si>
     <t>Bayes</t>
+  </si>
+  <si>
+    <t>requirement over random baseline</t>
   </si>
 </sst>
 </file>
@@ -865,8 +868,36 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="215">
+  <cellStyleXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -1088,7 +1119,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="215">
+  <cellStyles count="243">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -1196,6 +1227,20 @@
     <cellStyle name="Followed Hyperlink" xfId="210" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="212" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="214" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="216" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="218" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="220" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="222" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="224" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="226" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="228" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="230" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="232" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="234" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="236" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="238" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="240" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="242" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -1303,6 +1348,20 @@
     <cellStyle name="Hyperlink" xfId="209" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="211" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="213" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="215" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="217" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="219" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="221" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="223" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="225" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="227" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="229" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="231" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="233" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="235" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="237" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="239" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="241" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -7280,13 +7339,142 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C31" sqref="C31"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
-  <sheetData/>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>0.36399999999999999</v>
+      </c>
+      <c r="B3">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="C3">
+        <f>A3/B3</f>
+        <v>45.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>0.76</v>
+      </c>
+      <c r="B4">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C4">
+        <f t="shared" ref="C4:C12" si="0">A4/B4</f>
+        <v>152</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>0.93400000000000005</v>
+      </c>
+      <c r="B5">
+        <v>0.125</v>
+      </c>
+      <c r="C5">
+        <f t="shared" si="0"/>
+        <v>7.4720000000000004</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>0.38100000000000001</v>
+      </c>
+      <c r="B6">
+        <v>0.04</v>
+      </c>
+      <c r="C6">
+        <f t="shared" si="0"/>
+        <v>9.5250000000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>0.47599999999999998</v>
+      </c>
+      <c r="B7">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C7">
+        <f t="shared" si="0"/>
+        <v>68</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>9.0999999999999998E-2</v>
+      </c>
+      <c r="B8">
+        <v>4.2000000000000003E-2</v>
+      </c>
+      <c r="C8">
+        <f t="shared" si="0"/>
+        <v>2.1666666666666665</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>0.5</v>
+      </c>
+      <c r="B9">
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="C9">
+        <f t="shared" si="0"/>
+        <v>166.66666666666666</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>0.255</v>
+      </c>
+      <c r="B10">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C10">
+        <f t="shared" si="0"/>
+        <v>23.181818181818183</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="B11">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="C11">
+        <f t="shared" si="0"/>
+        <v>10.266666666666667</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>0.875</v>
+      </c>
+      <c r="B12">
+        <v>0.04</v>
+      </c>
+      <c r="C12">
+        <f t="shared" si="0"/>
+        <v>21.875</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -7299,7 +7487,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F73"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
+    <sheetView zoomScale="200" zoomScaleNormal="200" zoomScalePageLayoutView="200" workbookViewId="0">
       <selection activeCell="C65" sqref="C65"/>
     </sheetView>
   </sheetViews>
@@ -8441,7 +8629,7 @@
   <dimension ref="A1:G41"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H43" sqref="H43"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>

</xml_diff>